<commit_message>
Updated data collection sheet
</commit_message>
<xml_diff>
--- a/data/germination_data.xlsx
+++ b/data/germination_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanmeier/TELab/Soil Inoculation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanmeier/git/morasoilinoculation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07BE08F5-F88E-BD47-A246-9838ECA25A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59756CBC-EC68-8843-90F4-4344A6E7CCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="760" windowWidth="18080" windowHeight="17140" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
+    <workbookView xWindow="4420" yWindow="760" windowWidth="18080" windowHeight="17140" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="10">
   <si>
     <t>seed_species</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>inoculated_%</t>
+  </si>
+  <si>
+    <t>282_alive</t>
+  </si>
+  <si>
+    <t>282_dead</t>
   </si>
 </sst>
 </file>
@@ -121,13 +127,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:E212" totalsRowShown="0">
-  <autoFilter ref="B2:E212" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:G212" totalsRowShown="0">
+  <autoFilter ref="B2:G212" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1199D7AD-452C-9D4F-9453-306631F01BCC}" name="soil_species"/>
     <tableColumn id="2" xr3:uid="{11F49906-5A0D-4E4F-BA5C-F91CB62A2174}" name="seed_species"/>
     <tableColumn id="3" xr3:uid="{B695F4B4-8561-9D48-9FF3-12A40CB2B7C7}" name="inoculated_%"/>
     <tableColumn id="4" xr3:uid="{8A11EADE-C65F-784E-81F3-F09F807476AD}" name="notes"/>
+    <tableColumn id="5" xr3:uid="{51033E0C-19D6-5D44-8021-28156160EB71}" name="282_alive"/>
+    <tableColumn id="6" xr3:uid="{B3DB47D5-3D79-8044-9F36-AA1442CFD021}" name="282_dead"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68F8197-A530-A948-B005-AEDF71CF4B66}">
-  <dimension ref="B2:E212"/>
+  <dimension ref="B2:G212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +471,7 @@
     <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -476,8 +484,14 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -488,7 +502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -499,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -510,7 +524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -521,7 +535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -532,7 +546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -543,7 +557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -554,7 +568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -565,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -576,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -587,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -598,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -609,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -620,7 +634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
added first data to germination data sheet
</commit_message>
<xml_diff>
--- a/data/germination_data.xlsx
+++ b/data/germination_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanmeier/git/morasoilinoculation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94036523-FBFD-A24D-9761-328E4CDF7FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E692B52-4B3E-314E-BD8C-299476E9E105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="760" windowWidth="18080" windowHeight="17140" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="13">
   <si>
     <t>seed_species</t>
   </si>
@@ -62,13 +62,19 @@
     <t>inoculated_%</t>
   </si>
   <si>
-    <t>282_alive</t>
+    <t>pot</t>
   </si>
   <si>
-    <t>282_dead</t>
+    <t>296_alive</t>
   </si>
   <si>
-    <t>pot</t>
+    <t>296_dead</t>
+  </si>
+  <si>
+    <t>doy296: mold on soil</t>
+  </si>
+  <si>
+    <t>doy296: less mold on soil</t>
   </si>
 </sst>
 </file>
@@ -157,15 +163,31 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:H212" totalsRowShown="0">
-  <autoFilter ref="B2:H212" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}"/>
+  <autoFilter ref="B2:H212" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="THPL"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TSHE"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{1199D7AD-452C-9D4F-9453-306631F01BCC}" name="soil_species"/>
     <tableColumn id="2" xr3:uid="{11F49906-5A0D-4E4F-BA5C-F91CB62A2174}" name="seed_species"/>
     <tableColumn id="3" xr3:uid="{B695F4B4-8561-9D48-9FF3-12A40CB2B7C7}" name="inoculated_%"/>
     <tableColumn id="7" xr3:uid="{1DA27551-5E25-1241-A191-D3F866BA66FD}" name="pot"/>
     <tableColumn id="4" xr3:uid="{8A11EADE-C65F-784E-81F3-F09F807476AD}" name="notes"/>
-    <tableColumn id="5" xr3:uid="{51033E0C-19D6-5D44-8021-28156160EB71}" name="282_alive"/>
-    <tableColumn id="6" xr3:uid="{B3DB47D5-3D79-8044-9F36-AA1442CFD021}" name="282_dead"/>
+    <tableColumn id="5" xr3:uid="{51033E0C-19D6-5D44-8021-28156160EB71}" name="296_alive"/>
+    <tableColumn id="6" xr3:uid="{B3DB47D5-3D79-8044-9F36-AA1442CFD021}" name="296_dead"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -491,7 +513,7 @@
   <dimension ref="B2:H212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,19 +534,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -538,7 +560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -552,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -566,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -580,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -594,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -608,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -622,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -635,8 +657,11 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -647,6 +672,9 @@
         <v>10</v>
       </c>
       <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>1</v>
       </c>
     </row>
@@ -663,8 +691,11 @@
       <c r="E12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -678,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -691,8 +722,11 @@
       <c r="E14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -703,11 +737,11 @@
         <v>10</v>
       </c>
       <c r="E15" s="2">
-        <f>E3+1</f>
+        <f t="shared" ref="E15:E20" si="0">E3+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -718,11 +752,11 @@
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <f>E4+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -733,11 +767,11 @@
         <v>10</v>
       </c>
       <c r="E17" s="2">
-        <f>E5+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -748,11 +782,11 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f>E6+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -763,11 +797,11 @@
         <v>10</v>
       </c>
       <c r="E19" s="2">
-        <f>E7+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -778,11 +812,11 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <f>E8+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -796,7 +830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -807,11 +841,14 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <f>E10+1</f>
+        <f t="shared" ref="E22:E53" si="1">E10+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -822,11 +859,11 @@
         <v>10</v>
       </c>
       <c r="E23">
-        <f>E11+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -837,11 +874,14 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <f>E12+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -852,11 +892,11 @@
         <v>10</v>
       </c>
       <c r="E25">
-        <f>E13+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -867,11 +907,14 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <f>E14+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -882,11 +925,11 @@
         <v>10</v>
       </c>
       <c r="E27" s="2">
-        <f>E15+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -897,11 +940,11 @@
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <f>E16+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -912,11 +955,11 @@
         <v>10</v>
       </c>
       <c r="E29" s="2">
-        <f>E17+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -927,11 +970,14 @@
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <f>E18+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -942,11 +988,11 @@
         <v>10</v>
       </c>
       <c r="E31" s="2">
-        <f>E19+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -957,11 +1003,11 @@
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <f>E20+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -972,11 +1018,11 @@
         <v>10</v>
       </c>
       <c r="E33">
-        <f>E21+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -987,11 +1033,14 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <f>E22+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -1002,11 +1051,11 @@
         <v>10</v>
       </c>
       <c r="E35">
-        <f>E23+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -1017,11 +1066,14 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <f>E24+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -1032,11 +1084,11 @@
         <v>10</v>
       </c>
       <c r="E37">
-        <f>E25+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>4</v>
       </c>
@@ -1047,11 +1099,14 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <f>E26+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -1062,11 +1117,11 @@
         <v>10</v>
       </c>
       <c r="E39" s="2">
-        <f>E27+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -1077,11 +1132,11 @@
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <f>E28+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -1092,11 +1147,11 @@
         <v>10</v>
       </c>
       <c r="E41" s="2">
-        <f>E29+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -1107,11 +1162,14 @@
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <f>E30+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>1</v>
       </c>
@@ -1122,11 +1180,11 @@
         <v>10</v>
       </c>
       <c r="E43" s="2">
-        <f>E31+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>1</v>
       </c>
@@ -1137,11 +1195,11 @@
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <f>E32+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -1152,11 +1210,11 @@
         <v>10</v>
       </c>
       <c r="E45">
-        <f>E33+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>1</v>
       </c>
@@ -1167,11 +1225,14 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <f>E34+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -1182,11 +1243,11 @@
         <v>10</v>
       </c>
       <c r="E47">
-        <f>E35+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>4</v>
       </c>
@@ -1197,11 +1258,14 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <f>E36+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -1212,11 +1276,11 @@
         <v>10</v>
       </c>
       <c r="E49">
-        <f>E37+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -1227,11 +1291,14 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <f>E38+1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -1242,11 +1309,11 @@
         <v>10</v>
       </c>
       <c r="E51" s="2">
-        <f>E39+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -1257,11 +1324,11 @@
         <v>0</v>
       </c>
       <c r="E52" s="1">
-        <f>E40+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -1272,11 +1339,11 @@
         <v>10</v>
       </c>
       <c r="E53" s="2">
-        <f>E41+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -1287,11 +1354,11 @@
         <v>0</v>
       </c>
       <c r="E54" s="1">
-        <f>E42+1</f>
+        <f t="shared" ref="E54:E85" si="2">E42+1</f>
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>1</v>
       </c>
@@ -1302,11 +1369,11 @@
         <v>10</v>
       </c>
       <c r="E55" s="2">
-        <f>E43+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>1</v>
       </c>
@@ -1317,11 +1384,11 @@
         <v>0</v>
       </c>
       <c r="E56" s="1">
-        <f>E44+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -1332,11 +1399,11 @@
         <v>10</v>
       </c>
       <c r="E57">
-        <f>E45+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>1</v>
       </c>
@@ -1347,11 +1414,14 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <f>E46+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>4</v>
       </c>
@@ -1362,11 +1432,11 @@
         <v>10</v>
       </c>
       <c r="E59">
-        <f>E47+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>4</v>
       </c>
@@ -1377,11 +1447,14 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <f>E48+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>4</v>
       </c>
@@ -1392,11 +1465,11 @@
         <v>10</v>
       </c>
       <c r="E61">
-        <f>E49+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>4</v>
       </c>
@@ -1407,11 +1480,11 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <f>E50+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>3</v>
       </c>
@@ -1422,11 +1495,11 @@
         <v>10</v>
       </c>
       <c r="E63" s="2">
-        <f>E51+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>3</v>
       </c>
@@ -1437,11 +1510,11 @@
         <v>0</v>
       </c>
       <c r="E64" s="1">
-        <f>E52+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -1452,11 +1525,11 @@
         <v>10</v>
       </c>
       <c r="E65" s="2">
-        <f>E53+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>3</v>
       </c>
@@ -1467,11 +1540,11 @@
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <f>E54+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -1482,11 +1555,11 @@
         <v>10</v>
       </c>
       <c r="E67" s="2">
-        <f>E55+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -1497,11 +1570,11 @@
         <v>0</v>
       </c>
       <c r="E68" s="1">
-        <f>E56+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>1</v>
       </c>
@@ -1512,11 +1585,11 @@
         <v>10</v>
       </c>
       <c r="E69">
-        <f>E57+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>1</v>
       </c>
@@ -1527,11 +1600,14 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <f>E58+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>4</v>
       </c>
@@ -1542,11 +1618,11 @@
         <v>10</v>
       </c>
       <c r="E71">
-        <f>E59+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>4</v>
       </c>
@@ -1557,11 +1633,14 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <f>E60+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>4</v>
       </c>
@@ -1572,11 +1651,11 @@
         <v>10</v>
       </c>
       <c r="E73">
-        <f>E61+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>4</v>
       </c>
@@ -1587,11 +1666,14 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <f>E62+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>3</v>
       </c>
@@ -1602,11 +1684,11 @@
         <v>10</v>
       </c>
       <c r="E75" s="2">
-        <f>E63+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>3</v>
       </c>
@@ -1617,11 +1699,11 @@
         <v>0</v>
       </c>
       <c r="E76" s="1">
-        <f>E64+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>3</v>
       </c>
@@ -1632,11 +1714,11 @@
         <v>10</v>
       </c>
       <c r="E77" s="2">
-        <f>E65+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>3</v>
       </c>
@@ -1647,11 +1729,14 @@
         <v>0</v>
       </c>
       <c r="E78" s="1">
-        <f>E66+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>1</v>
       </c>
@@ -1662,11 +1747,11 @@
         <v>10</v>
       </c>
       <c r="E79" s="2">
-        <f>E67+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>1</v>
       </c>
@@ -1677,11 +1762,11 @@
         <v>0</v>
       </c>
       <c r="E80" s="1">
-        <f>E68+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>1</v>
       </c>
@@ -1692,11 +1777,11 @@
         <v>10</v>
       </c>
       <c r="E81">
-        <f>E69+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>1</v>
       </c>
@@ -1707,11 +1792,14 @@
         <v>0</v>
       </c>
       <c r="E82">
-        <f>E70+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>4</v>
       </c>
@@ -1722,11 +1810,11 @@
         <v>10</v>
       </c>
       <c r="E83">
-        <f>E71+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>4</v>
       </c>
@@ -1737,11 +1825,14 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <f>E72+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>4</v>
       </c>
@@ -1752,11 +1843,11 @@
         <v>10</v>
       </c>
       <c r="E85">
-        <f>E73+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>4</v>
       </c>
@@ -1767,11 +1858,14 @@
         <v>0</v>
       </c>
       <c r="E86">
-        <f>E74+1</f>
+        <f t="shared" ref="E86:E117" si="3">E74+1</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>3</v>
       </c>
@@ -1782,11 +1876,11 @@
         <v>10</v>
       </c>
       <c r="E87" s="2">
-        <f>E75+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>3</v>
       </c>
@@ -1797,11 +1891,11 @@
         <v>0</v>
       </c>
       <c r="E88" s="1">
-        <f>E76+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>3</v>
       </c>
@@ -1812,11 +1906,11 @@
         <v>10</v>
       </c>
       <c r="E89" s="2">
-        <f>E77+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>3</v>
       </c>
@@ -1827,11 +1921,11 @@
         <v>0</v>
       </c>
       <c r="E90" s="1">
-        <f>E78+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>1</v>
       </c>
@@ -1842,11 +1936,11 @@
         <v>10</v>
       </c>
       <c r="E91" s="2">
-        <f>E79+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>1</v>
       </c>
@@ -1857,11 +1951,11 @@
         <v>0</v>
       </c>
       <c r="E92" s="1">
-        <f>E80+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>1</v>
       </c>
@@ -1872,11 +1966,11 @@
         <v>10</v>
       </c>
       <c r="E93">
-        <f>E81+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>1</v>
       </c>
@@ -1887,11 +1981,14 @@
         <v>0</v>
       </c>
       <c r="E94">
-        <f>E82+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>4</v>
       </c>
@@ -1902,11 +1999,11 @@
         <v>10</v>
       </c>
       <c r="E95">
-        <f>E83+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>4</v>
       </c>
@@ -1917,11 +2014,14 @@
         <v>0</v>
       </c>
       <c r="E96">
-        <f>E84+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F96" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>4</v>
       </c>
@@ -1932,11 +2032,11 @@
         <v>10</v>
       </c>
       <c r="E97">
-        <f>E85+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>4</v>
       </c>
@@ -1947,11 +2047,14 @@
         <v>0</v>
       </c>
       <c r="E98">
-        <f>E86+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>3</v>
       </c>
@@ -1962,11 +2065,11 @@
         <v>10</v>
       </c>
       <c r="E99" s="2">
-        <f>E87+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>3</v>
       </c>
@@ -1977,11 +2080,11 @@
         <v>0</v>
       </c>
       <c r="E100" s="1">
-        <f>E88+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>3</v>
       </c>
@@ -1992,11 +2095,11 @@
         <v>10</v>
       </c>
       <c r="E101" s="2">
-        <f>E89+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>3</v>
       </c>
@@ -2007,11 +2110,11 @@
         <v>0</v>
       </c>
       <c r="E102" s="1">
-        <f>E90+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>1</v>
       </c>
@@ -2022,11 +2125,11 @@
         <v>10</v>
       </c>
       <c r="E103" s="2">
-        <f>E91+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>1</v>
       </c>
@@ -2037,11 +2140,11 @@
         <v>0</v>
       </c>
       <c r="E104" s="1">
-        <f>E92+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>1</v>
       </c>
@@ -2052,11 +2155,11 @@
         <v>10</v>
       </c>
       <c r="E105">
-        <f>E93+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>1</v>
       </c>
@@ -2067,11 +2170,14 @@
         <v>0</v>
       </c>
       <c r="E106">
-        <f>E94+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F106" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>4</v>
       </c>
@@ -2082,11 +2188,11 @@
         <v>10</v>
       </c>
       <c r="E107">
-        <f>E95+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>4</v>
       </c>
@@ -2097,11 +2203,14 @@
         <v>0</v>
       </c>
       <c r="E108">
-        <f>E96+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F108" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>4</v>
       </c>
@@ -2112,11 +2221,11 @@
         <v>10</v>
       </c>
       <c r="E109">
-        <f>E97+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>4</v>
       </c>
@@ -2127,11 +2236,14 @@
         <v>0</v>
       </c>
       <c r="E110">
-        <f>E98+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F110" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>3</v>
       </c>
@@ -2142,11 +2254,14 @@
         <v>10</v>
       </c>
       <c r="E111" s="2">
-        <f>E99+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>3</v>
       </c>
@@ -2157,11 +2272,11 @@
         <v>0</v>
       </c>
       <c r="E112" s="1">
-        <f>E100+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>3</v>
       </c>
@@ -2172,11 +2287,11 @@
         <v>10</v>
       </c>
       <c r="E113" s="2">
-        <f>E101+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>3</v>
       </c>
@@ -2187,11 +2302,11 @@
         <v>0</v>
       </c>
       <c r="E114" s="1">
-        <f>E102+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>1</v>
       </c>
@@ -2202,11 +2317,11 @@
         <v>10</v>
       </c>
       <c r="E115" s="2">
-        <f>E103+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>1</v>
       </c>
@@ -2217,11 +2332,11 @@
         <v>0</v>
       </c>
       <c r="E116" s="1">
-        <f>E104+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>1</v>
       </c>
@@ -2232,11 +2347,11 @@
         <v>10</v>
       </c>
       <c r="E117">
-        <f>E105+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>1</v>
       </c>
@@ -2247,11 +2362,12 @@
         <v>0</v>
       </c>
       <c r="E118">
-        <f>E106+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" ref="E118:E149" si="4">E106+1</f>
+        <v>10</v>
+      </c>
+      <c r="F118" s="1"/>
+    </row>
+    <row r="119" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>4</v>
       </c>
@@ -2262,11 +2378,11 @@
         <v>10</v>
       </c>
       <c r="E119">
-        <f>E107+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>4</v>
       </c>
@@ -2277,11 +2393,14 @@
         <v>0</v>
       </c>
       <c r="E120">
-        <f>E108+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="F120" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>4</v>
       </c>
@@ -2292,11 +2411,11 @@
         <v>10</v>
       </c>
       <c r="E121">
-        <f>E109+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>4</v>
       </c>
@@ -2307,11 +2426,14 @@
         <v>0</v>
       </c>
       <c r="E122">
-        <f>E110+1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -2322,11 +2444,11 @@
         <v>10</v>
       </c>
       <c r="E123" s="2">
-        <f>E111+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>3</v>
       </c>
@@ -2337,11 +2459,11 @@
         <v>0</v>
       </c>
       <c r="E124" s="1">
-        <f>E112+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>3</v>
       </c>
@@ -2352,11 +2474,11 @@
         <v>10</v>
       </c>
       <c r="E125" s="2">
-        <f>E113+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>3</v>
       </c>
@@ -2367,11 +2489,11 @@
         <v>0</v>
       </c>
       <c r="E126" s="1">
-        <f>E114+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>1</v>
       </c>
@@ -2382,11 +2504,11 @@
         <v>10</v>
       </c>
       <c r="E127" s="2">
-        <f>E115+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>1</v>
       </c>
@@ -2397,11 +2519,11 @@
         <v>0</v>
       </c>
       <c r="E128" s="1">
-        <f>E116+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>1</v>
       </c>
@@ -2412,11 +2534,11 @@
         <v>10</v>
       </c>
       <c r="E129">
-        <f>E117+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>1</v>
       </c>
@@ -2427,11 +2549,14 @@
         <v>0</v>
       </c>
       <c r="E130">
-        <f>E118+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>4</v>
       </c>
@@ -2442,11 +2567,11 @@
         <v>10</v>
       </c>
       <c r="E131">
-        <f>E119+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>4</v>
       </c>
@@ -2457,11 +2582,14 @@
         <v>0</v>
       </c>
       <c r="E132">
-        <f>E120+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="F132" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>4</v>
       </c>
@@ -2472,11 +2600,11 @@
         <v>10</v>
       </c>
       <c r="E133">
-        <f>E121+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>4</v>
       </c>
@@ -2487,11 +2615,14 @@
         <v>0</v>
       </c>
       <c r="E134">
-        <f>E122+1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>3</v>
       </c>
@@ -2502,11 +2633,11 @@
         <v>10</v>
       </c>
       <c r="E135" s="2">
-        <f>E123+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>3</v>
       </c>
@@ -2517,11 +2648,11 @@
         <v>0</v>
       </c>
       <c r="E136" s="1">
-        <f>E124+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>3</v>
       </c>
@@ -2532,11 +2663,11 @@
         <v>10</v>
       </c>
       <c r="E137" s="2">
-        <f>E125+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>3</v>
       </c>
@@ -2547,11 +2678,11 @@
         <v>0</v>
       </c>
       <c r="E138" s="1">
-        <f>E126+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>1</v>
       </c>
@@ -2562,11 +2693,11 @@
         <v>10</v>
       </c>
       <c r="E139" s="2">
-        <f>E127+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>1</v>
       </c>
@@ -2577,11 +2708,11 @@
         <v>0</v>
       </c>
       <c r="E140" s="1">
-        <f>E128+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>1</v>
       </c>
@@ -2592,11 +2723,11 @@
         <v>10</v>
       </c>
       <c r="E141">
-        <f>E129+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>1</v>
       </c>
@@ -2607,11 +2738,14 @@
         <v>0</v>
       </c>
       <c r="E142">
-        <f>E130+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F142" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>4</v>
       </c>
@@ -2622,11 +2756,11 @@
         <v>10</v>
       </c>
       <c r="E143">
-        <f>E131+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>4</v>
       </c>
@@ -2637,11 +2771,14 @@
         <v>0</v>
       </c>
       <c r="E144">
-        <f>E132+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F144" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>4</v>
       </c>
@@ -2652,11 +2789,11 @@
         <v>10</v>
       </c>
       <c r="E145">
-        <f>E133+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>4</v>
       </c>
@@ -2667,11 +2804,14 @@
         <v>0</v>
       </c>
       <c r="E146">
-        <f>E134+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F146" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>3</v>
       </c>
@@ -2682,11 +2822,11 @@
         <v>10</v>
       </c>
       <c r="E147" s="2">
-        <f>E135+1</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>3</v>
       </c>
@@ -2697,11 +2837,11 @@
         <v>0</v>
       </c>
       <c r="E148" s="1">
-        <f>E136+1</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>3</v>
       </c>
@@ -2712,11 +2852,11 @@
         <v>10</v>
       </c>
       <c r="E149" s="2">
-        <f>E137+1</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>3</v>
       </c>
@@ -2727,11 +2867,14 @@
         <v>0</v>
       </c>
       <c r="E150" s="1">
-        <f>E138+1</f>
+        <f t="shared" ref="E150:E181" si="5">E138+1</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F150" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>1</v>
       </c>
@@ -2742,11 +2885,11 @@
         <v>10</v>
       </c>
       <c r="E151" s="2">
-        <f>E139+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>1</v>
       </c>
@@ -2757,11 +2900,11 @@
         <v>0</v>
       </c>
       <c r="E152" s="1">
-        <f>E140+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>1</v>
       </c>
@@ -2772,11 +2915,11 @@
         <v>10</v>
       </c>
       <c r="E153">
-        <f>E141+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>1</v>
       </c>
@@ -2787,11 +2930,14 @@
         <v>0</v>
       </c>
       <c r="E154">
-        <f>E142+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F154" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>4</v>
       </c>
@@ -2802,11 +2948,11 @@
         <v>10</v>
       </c>
       <c r="E155">
-        <f>E143+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>4</v>
       </c>
@@ -2817,11 +2963,14 @@
         <v>0</v>
       </c>
       <c r="E156">
-        <f>E144+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F156" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>4</v>
       </c>
@@ -2832,11 +2981,11 @@
         <v>10</v>
       </c>
       <c r="E157">
-        <f>E145+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>4</v>
       </c>
@@ -2847,11 +2996,14 @@
         <v>0</v>
       </c>
       <c r="E158">
-        <f>E146+1</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F158" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>3</v>
       </c>
@@ -2862,11 +3014,11 @@
         <v>10</v>
       </c>
       <c r="E159" s="2">
-        <f>E147+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>3</v>
       </c>
@@ -2877,11 +3029,11 @@
         <v>0</v>
       </c>
       <c r="E160" s="1">
-        <f>E148+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>3</v>
       </c>
@@ -2892,11 +3044,11 @@
         <v>10</v>
       </c>
       <c r="E161" s="2">
-        <f>E149+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>3</v>
       </c>
@@ -2907,11 +3059,11 @@
         <v>0</v>
       </c>
       <c r="E162" s="1">
-        <f>E150+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>1</v>
       </c>
@@ -2922,11 +3074,11 @@
         <v>10</v>
       </c>
       <c r="E163" s="2">
-        <f>E151+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>1</v>
       </c>
@@ -2937,11 +3089,11 @@
         <v>0</v>
       </c>
       <c r="E164" s="1">
-        <f>E152+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>1</v>
       </c>
@@ -2952,11 +3104,11 @@
         <v>10</v>
       </c>
       <c r="E165">
-        <f>E153+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>1</v>
       </c>
@@ -2967,11 +3119,14 @@
         <v>0</v>
       </c>
       <c r="E166">
-        <f>E154+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F166" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>4</v>
       </c>
@@ -2982,11 +3137,11 @@
         <v>10</v>
       </c>
       <c r="E167">
-        <f>E155+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>4</v>
       </c>
@@ -2997,11 +3152,14 @@
         <v>0</v>
       </c>
       <c r="E168">
-        <f>E156+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F168" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>4</v>
       </c>
@@ -3012,11 +3170,11 @@
         <v>10</v>
       </c>
       <c r="E169">
-        <f>E157+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>4</v>
       </c>
@@ -3027,11 +3185,11 @@
         <v>0</v>
       </c>
       <c r="E170">
-        <f>E158+1</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>3</v>
       </c>
@@ -3042,11 +3200,11 @@
         <v>10</v>
       </c>
       <c r="E171" s="2">
-        <f>E159+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>3</v>
       </c>
@@ -3057,11 +3215,11 @@
         <v>0</v>
       </c>
       <c r="E172" s="1">
-        <f>E160+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>3</v>
       </c>
@@ -3072,11 +3230,11 @@
         <v>10</v>
       </c>
       <c r="E173" s="2">
-        <f>E161+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>3</v>
       </c>
@@ -3087,11 +3245,11 @@
         <v>0</v>
       </c>
       <c r="E174" s="1">
-        <f>E162+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>1</v>
       </c>
@@ -3102,11 +3260,11 @@
         <v>10</v>
       </c>
       <c r="E175" s="2">
-        <f>E163+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>1</v>
       </c>
@@ -3117,11 +3275,11 @@
         <v>0</v>
       </c>
       <c r="E176" s="1">
-        <f>E164+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>1</v>
       </c>
@@ -3132,11 +3290,11 @@
         <v>10</v>
       </c>
       <c r="E177">
-        <f>E165+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>1</v>
       </c>
@@ -3147,11 +3305,14 @@
         <v>0</v>
       </c>
       <c r="E178">
-        <f>E166+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="179" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F178" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>4</v>
       </c>
@@ -3162,11 +3323,11 @@
         <v>10</v>
       </c>
       <c r="E179">
-        <f>E167+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>4</v>
       </c>
@@ -3177,11 +3338,14 @@
         <v>0</v>
       </c>
       <c r="E180">
-        <f>E168+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="181" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F180" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>4</v>
       </c>
@@ -3192,11 +3356,11 @@
         <v>10</v>
       </c>
       <c r="E181">
-        <f>E169+1</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>4</v>
       </c>
@@ -3207,11 +3371,11 @@
         <v>0</v>
       </c>
       <c r="E182">
-        <f>E170+1</f>
+        <f t="shared" ref="E182:E213" si="6">E170+1</f>
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>3</v>
       </c>
@@ -3225,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>1</v>
       </c>
@@ -3239,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>3</v>
       </c>
@@ -3253,7 +3417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>1</v>
       </c>
@@ -3267,7 +3431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>4</v>
       </c>
@@ -3281,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>4</v>
       </c>
@@ -3295,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>3</v>
       </c>
@@ -3309,7 +3473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>1</v>
       </c>
@@ -3323,7 +3487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>3</v>
       </c>
@@ -3337,7 +3501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>1</v>
       </c>
@@ -3351,7 +3515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>4</v>
       </c>
@@ -3365,7 +3529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>4</v>
       </c>
@@ -3379,7 +3543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>3</v>
       </c>
@@ -3393,7 +3557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>1</v>
       </c>
@@ -3407,7 +3571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>3</v>
       </c>
@@ -3421,7 +3585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>1</v>
       </c>
@@ -3435,7 +3599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>4</v>
       </c>
@@ -3449,7 +3613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>4</v>
       </c>
@@ -3463,7 +3627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>3</v>
       </c>
@@ -3477,7 +3641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>1</v>
       </c>
@@ -3491,7 +3655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
         <v>3</v>
       </c>
@@ -3505,7 +3669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
         <v>1</v>
       </c>
@@ -3519,7 +3683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
         <v>4</v>
       </c>
@@ -3533,7 +3697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
         <v>4</v>
       </c>
@@ -3547,7 +3711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
         <v>3</v>
       </c>
@@ -3561,7 +3725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
         <v>1</v>
       </c>
@@ -3575,7 +3739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
         <v>3</v>
       </c>
@@ -3589,7 +3753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
         <v>1</v>
       </c>
@@ -3603,7 +3767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
         <v>4</v>
       </c>
@@ -3617,7 +3781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
germ data for DOY314
</commit_message>
<xml_diff>
--- a/data/germination_data.xlsx
+++ b/data/germination_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanmeier/git/morasoilinoculation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\morasoilinoculation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206F45BA-2034-9B45-A6DB-28682F32757C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29FD187-D84F-44EC-90FB-C3A5D7404ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="760" windowWidth="18080" windowHeight="17140" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="33">
   <si>
     <t>seed_species</t>
   </si>
@@ -130,6 +130,14 @@
   <si>
     <t>doy310: one germinant alive but uprooted</t>
   </si>
+  <si>
+    <t>314_alive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>314_dead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -139,20 +147,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -216,25 +224,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:P213" totalsRowShown="0">
-  <autoFilter ref="B2:P213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="TSHE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TSHE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="10"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:R213" totalsRowShown="0">
+  <autoFilter ref="B2:R213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{1199D7AD-452C-9D4F-9453-306631F01BCC}" name="soil_species"/>
     <tableColumn id="2" xr3:uid="{11F49906-5A0D-4E4F-BA5C-F91CB62A2174}" name="seed_species"/>
     <tableColumn id="3" xr3:uid="{B695F4B4-8561-9D48-9FF3-12A40CB2B7C7}" name="inoculated_%"/>
@@ -250,6 +242,8 @@
     <tableColumn id="13" xr3:uid="{F54096F7-8245-934E-86A0-6F0E698FAA54}" name="307_dead"/>
     <tableColumn id="14" xr3:uid="{CB213D8E-3305-D040-90CC-DE1DDB3275C4}" name="310_alive"/>
     <tableColumn id="15" xr3:uid="{4AC10E25-3833-6A46-9112-7B9EE97738A4}" name="310_dead"/>
+    <tableColumn id="16" xr3:uid="{61FD7D15-B811-4B50-B1A4-3307C6CFBD54}" name="314_alive"/>
+    <tableColumn id="17" xr3:uid="{D3CF8275-7C0E-40DB-8D90-3B1CFB4C2521}" name="314_dead"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -572,20 +566,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68F8197-A530-A948-B005-AEDF71CF4B66}">
-  <dimension ref="B2:P213"/>
+  <dimension ref="B2:R212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="O214" sqref="O214"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.15234375" customWidth="1"/>
+    <col min="4" max="4" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -631,8 +625,14 @@
       <c r="P2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -651,8 +651,11 @@
       <c r="O3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -671,8 +674,11 @@
       <c r="O4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -691,8 +697,11 @@
       <c r="O5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -714,8 +723,11 @@
       <c r="O6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -731,8 +743,11 @@
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -745,8 +760,11 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -768,8 +786,11 @@
       <c r="O9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -794,8 +815,11 @@
       <c r="O10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -817,8 +841,11 @@
       <c r="O11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -837,8 +864,11 @@
       <c r="O12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -860,8 +890,11 @@
       <c r="O13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -892,8 +925,14 @@
       <c r="P14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -913,8 +952,11 @@
       <c r="O15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -934,8 +976,11 @@
       <c r="O16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -958,8 +1003,11 @@
       <c r="O17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -976,8 +1024,11 @@
       <c r="M18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -991,8 +1042,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -1006,8 +1060,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -1026,8 +1083,11 @@
       <c r="O21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -1050,8 +1110,11 @@
       <c r="M22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -1068,8 +1131,11 @@
       <c r="K23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -1089,8 +1155,11 @@
       <c r="M24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -1110,8 +1179,11 @@
       <c r="M25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -1146,8 +1218,14 @@
       <c r="P26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q26">
+        <v>6</v>
+      </c>
+      <c r="R26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -1167,8 +1245,11 @@
       <c r="O27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -1188,8 +1269,11 @@
       <c r="O28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -1209,8 +1293,11 @@
       <c r="O29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -1236,8 +1323,11 @@
       <c r="O30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -1254,8 +1344,11 @@
       <c r="O31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -1269,8 +1362,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -1293,8 +1389,11 @@
       <c r="O33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -1323,8 +1422,11 @@
       <c r="O34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -1341,8 +1443,11 @@
       <c r="O35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -1362,8 +1467,11 @@
       <c r="O36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -1383,8 +1491,11 @@
       <c r="O37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>4</v>
       </c>
@@ -1416,8 +1527,14 @@
       <c r="P38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q38">
+        <v>3</v>
+      </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -1437,8 +1554,11 @@
       <c r="O39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -1458,8 +1578,14 @@
       <c r="O40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -1479,8 +1605,11 @@
       <c r="O41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -1509,8 +1638,11 @@
       <c r="O42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>1</v>
       </c>
@@ -1527,8 +1659,11 @@
       <c r="O43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>1</v>
       </c>
@@ -1542,8 +1677,11 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -1578,8 +1716,14 @@
       <c r="P45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q45">
+        <v>6</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>1</v>
       </c>
@@ -1605,8 +1749,11 @@
       <c r="O46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -1623,8 +1770,11 @@
       <c r="O47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>4</v>
       </c>
@@ -1647,8 +1797,11 @@
       <c r="O48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -1668,8 +1821,11 @@
       <c r="O49">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -1704,8 +1860,14 @@
       <c r="P50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q50">
+        <v>5</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -1725,8 +1887,11 @@
       <c r="O51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -1746,8 +1911,11 @@
       <c r="O52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -1767,8 +1935,11 @@
       <c r="O53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -1791,8 +1962,11 @@
       <c r="O54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>1</v>
       </c>
@@ -1809,8 +1983,11 @@
       <c r="O55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>1</v>
       </c>
@@ -1824,8 +2001,11 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -1845,8 +2025,11 @@
       <c r="O57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>1</v>
       </c>
@@ -1872,8 +2055,11 @@
       <c r="O58">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>4</v>
       </c>
@@ -1890,8 +2076,11 @@
       <c r="O59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>4</v>
       </c>
@@ -1911,8 +2100,11 @@
       <c r="O60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>4</v>
       </c>
@@ -1932,8 +2124,11 @@
       <c r="O61">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>4</v>
       </c>
@@ -1965,8 +2160,14 @@
       <c r="P62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q62">
+        <v>3</v>
+      </c>
+      <c r="R62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>3</v>
       </c>
@@ -1986,8 +2187,11 @@
       <c r="O63">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>3</v>
       </c>
@@ -2007,8 +2211,14 @@
       <c r="O64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q64">
+        <v>4</v>
+      </c>
+      <c r="R64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -2028,8 +2238,11 @@
       <c r="O65">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>3</v>
       </c>
@@ -2049,8 +2262,11 @@
       <c r="O66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -2067,8 +2283,11 @@
       <c r="O67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -2082,8 +2301,11 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>1</v>
       </c>
@@ -2103,8 +2325,11 @@
       <c r="O69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>1</v>
       </c>
@@ -2133,8 +2358,11 @@
       <c r="O70">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>4</v>
       </c>
@@ -2151,8 +2379,11 @@
       <c r="O71">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q71">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>4</v>
       </c>
@@ -2172,8 +2403,11 @@
       <c r="O72">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>4</v>
       </c>
@@ -2193,8 +2427,11 @@
       <c r="O73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>4</v>
       </c>
@@ -2223,8 +2460,11 @@
       <c r="O74">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>3</v>
       </c>
@@ -2244,8 +2484,11 @@
       <c r="O75">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>3</v>
       </c>
@@ -2265,8 +2508,11 @@
       <c r="O76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>3</v>
       </c>
@@ -2289,8 +2535,11 @@
       <c r="O77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>3</v>
       </c>
@@ -2313,8 +2562,11 @@
       <c r="O78">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>1</v>
       </c>
@@ -2334,8 +2586,11 @@
       <c r="O79">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>1</v>
       </c>
@@ -2349,8 +2604,11 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>1</v>
       </c>
@@ -2376,8 +2634,11 @@
       <c r="O81">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>1</v>
       </c>
@@ -2403,8 +2664,11 @@
       <c r="O82">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q82">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>4</v>
       </c>
@@ -2421,8 +2685,11 @@
       <c r="O83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>4</v>
       </c>
@@ -2442,8 +2709,11 @@
       <c r="O84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>4</v>
       </c>
@@ -2463,8 +2733,11 @@
       <c r="O85">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>4</v>
       </c>
@@ -2493,8 +2766,11 @@
       <c r="O86">
         <v>8</v>
       </c>
-    </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q86">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>3</v>
       </c>
@@ -2514,8 +2790,11 @@
       <c r="O87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>3</v>
       </c>
@@ -2535,8 +2814,11 @@
       <c r="O88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>3</v>
       </c>
@@ -2559,8 +2841,11 @@
       <c r="O89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>3</v>
       </c>
@@ -2583,8 +2868,11 @@
       <c r="O90">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q90">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>1</v>
       </c>
@@ -2604,8 +2892,11 @@
       <c r="O91">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>1</v>
       </c>
@@ -2619,8 +2910,11 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="93" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>1</v>
       </c>
@@ -2643,8 +2937,11 @@
       <c r="O93">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>1</v>
       </c>
@@ -2670,8 +2967,11 @@
       <c r="O94">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>4</v>
       </c>
@@ -2688,8 +2988,11 @@
       <c r="O95">
         <v>2</v>
       </c>
-    </row>
-    <row r="96" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>4</v>
       </c>
@@ -2709,8 +3012,11 @@
       <c r="O96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>4</v>
       </c>
@@ -2733,8 +3039,11 @@
       <c r="O97">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>4</v>
       </c>
@@ -2760,8 +3069,11 @@
       <c r="O98">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>3</v>
       </c>
@@ -2778,8 +3090,11 @@
       <c r="O99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>3</v>
       </c>
@@ -2799,8 +3114,11 @@
       <c r="O100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>3</v>
       </c>
@@ -2820,8 +3138,11 @@
       <c r="O101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>3</v>
       </c>
@@ -2844,8 +3165,11 @@
       <c r="O102">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q102">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>1</v>
       </c>
@@ -2859,8 +3183,11 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>1</v>
       </c>
@@ -2874,8 +3201,11 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>1</v>
       </c>
@@ -2895,8 +3225,11 @@
       <c r="O105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>1</v>
       </c>
@@ -2922,8 +3255,11 @@
       <c r="O106">
         <v>3</v>
       </c>
-    </row>
-    <row r="107" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>4</v>
       </c>
@@ -2937,8 +3273,11 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>4</v>
       </c>
@@ -2955,8 +3294,11 @@
       <c r="F108" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="109" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>4</v>
       </c>
@@ -2976,8 +3318,11 @@
       <c r="O109">
         <v>7</v>
       </c>
-    </row>
-    <row r="110" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>4</v>
       </c>
@@ -3006,8 +3351,11 @@
       <c r="O110">
         <v>6</v>
       </c>
-    </row>
-    <row r="111" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q110">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>3</v>
       </c>
@@ -3030,8 +3378,11 @@
       <c r="O111">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>3</v>
       </c>
@@ -3051,8 +3402,11 @@
       <c r="O112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>3</v>
       </c>
@@ -3072,8 +3426,11 @@
       <c r="O113">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>3</v>
       </c>
@@ -3096,8 +3453,11 @@
       <c r="O114">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>1</v>
       </c>
@@ -3114,8 +3474,11 @@
       <c r="O115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>1</v>
       </c>
@@ -3129,8 +3492,11 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="117" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>1</v>
       </c>
@@ -3150,8 +3516,11 @@
       <c r="O117">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q117">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>1</v>
       </c>
@@ -3178,8 +3547,11 @@
       <c r="O118">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>4</v>
       </c>
@@ -3196,8 +3568,11 @@
       <c r="O119">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>4</v>
       </c>
@@ -3217,8 +3592,11 @@
       <c r="O120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>4</v>
       </c>
@@ -3238,8 +3616,11 @@
       <c r="O121">
         <v>6</v>
       </c>
-    </row>
-    <row r="122" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q121">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>4</v>
       </c>
@@ -3265,8 +3646,11 @@
       <c r="O122">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -3286,8 +3670,11 @@
       <c r="O123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>3</v>
       </c>
@@ -3310,8 +3697,11 @@
       <c r="O124">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q124">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>3</v>
       </c>
@@ -3331,8 +3721,11 @@
       <c r="O125">
         <v>3</v>
       </c>
-    </row>
-    <row r="126" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q125">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>3</v>
       </c>
@@ -3355,8 +3748,11 @@
       <c r="O126">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>1</v>
       </c>
@@ -3370,8 +3766,11 @@
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="128" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>1</v>
       </c>
@@ -3385,8 +3784,11 @@
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="129" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>1</v>
       </c>
@@ -3409,8 +3811,14 @@
       <c r="O129">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q129">
+        <v>5</v>
+      </c>
+      <c r="R129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>1</v>
       </c>
@@ -3436,8 +3844,11 @@
       <c r="O130">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q130">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>4</v>
       </c>
@@ -3451,8 +3862,11 @@
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="132" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>4</v>
       </c>
@@ -3469,8 +3883,11 @@
       <c r="F132" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="133" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>4</v>
       </c>
@@ -3490,8 +3907,11 @@
       <c r="O133">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q133">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
         <v>4</v>
       </c>
@@ -3520,8 +3940,11 @@
       <c r="O134">
         <v>7</v>
       </c>
-    </row>
-    <row r="135" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q134">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
         <v>3</v>
       </c>
@@ -3541,8 +3964,11 @@
       <c r="O135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q135">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
         <v>3</v>
       </c>
@@ -3562,8 +3988,11 @@
       <c r="O136">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
         <v>3</v>
       </c>
@@ -3586,8 +4015,11 @@
       <c r="O137">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q137">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
         <v>3</v>
       </c>
@@ -3610,8 +4042,11 @@
       <c r="O138">
         <v>6</v>
       </c>
-    </row>
-    <row r="139" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q138">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
         <v>1</v>
       </c>
@@ -3625,8 +4060,11 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="140" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
         <v>1</v>
       </c>
@@ -3640,8 +4078,11 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="141" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
         <v>1</v>
       </c>
@@ -3667,8 +4108,14 @@
       <c r="O141">
         <v>7</v>
       </c>
-    </row>
-    <row r="142" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q141">
+        <v>6</v>
+      </c>
+      <c r="R141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>1</v>
       </c>
@@ -3694,8 +4141,11 @@
       <c r="O142">
         <v>7</v>
       </c>
-    </row>
-    <row r="143" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q142">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>4</v>
       </c>
@@ -3709,8 +4159,11 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="144" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>4</v>
       </c>
@@ -3727,8 +4180,11 @@
       <c r="F144" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="145" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>4</v>
       </c>
@@ -3751,8 +4207,11 @@
       <c r="O145">
         <v>6</v>
       </c>
-    </row>
-    <row r="146" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q145">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>4</v>
       </c>
@@ -3781,8 +4240,11 @@
       <c r="O146">
         <v>7</v>
       </c>
-    </row>
-    <row r="147" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q146">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>3</v>
       </c>
@@ -3799,8 +4261,11 @@
       <c r="O147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>3</v>
       </c>
@@ -3820,8 +4285,11 @@
       <c r="O148">
         <v>2</v>
       </c>
-    </row>
-    <row r="149" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q148">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>3</v>
       </c>
@@ -3841,8 +4309,11 @@
       <c r="O149">
         <v>3</v>
       </c>
-    </row>
-    <row r="150" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>3</v>
       </c>
@@ -3868,8 +4339,11 @@
       <c r="O150">
         <v>4</v>
       </c>
-    </row>
-    <row r="151" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q150">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
         <v>1</v>
       </c>
@@ -3883,8 +4357,11 @@
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="152" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
         <v>1</v>
       </c>
@@ -3898,8 +4375,11 @@
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="153" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
         <v>1</v>
       </c>
@@ -3919,8 +4399,11 @@
       <c r="O153">
         <v>3</v>
       </c>
-    </row>
-    <row r="154" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q153">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
         <v>1</v>
       </c>
@@ -3946,8 +4429,14 @@
       <c r="O154">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q154">
+        <v>1</v>
+      </c>
+      <c r="R154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
         <v>4</v>
       </c>
@@ -3961,8 +4450,11 @@
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="156" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
         <v>4</v>
       </c>
@@ -3982,8 +4474,11 @@
       <c r="O156">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
         <v>4</v>
       </c>
@@ -4003,8 +4498,11 @@
       <c r="O157">
         <v>3</v>
       </c>
-    </row>
-    <row r="158" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B158" t="s">
         <v>4</v>
       </c>
@@ -4033,8 +4531,11 @@
       <c r="O158">
         <v>6</v>
       </c>
-    </row>
-    <row r="159" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q158">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B159" t="s">
         <v>3</v>
       </c>
@@ -4051,8 +4552,11 @@
       <c r="O159">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B160" t="s">
         <v>3</v>
       </c>
@@ -4072,8 +4576,11 @@
       <c r="O160">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q160">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B161" t="s">
         <v>3</v>
       </c>
@@ -4093,8 +4600,11 @@
       <c r="O161">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q161">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
         <v>3</v>
       </c>
@@ -4117,8 +4627,11 @@
       <c r="O162">
         <v>7</v>
       </c>
-    </row>
-    <row r="163" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q162">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>1</v>
       </c>
@@ -4132,8 +4645,11 @@
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="164" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>1</v>
       </c>
@@ -4147,8 +4663,11 @@
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="165" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q164">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>1</v>
       </c>
@@ -4168,8 +4687,11 @@
       <c r="O165">
         <v>3</v>
       </c>
-    </row>
-    <row r="166" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>1</v>
       </c>
@@ -4195,8 +4717,11 @@
       <c r="O166">
         <v>4</v>
       </c>
-    </row>
-    <row r="167" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
         <v>4</v>
       </c>
@@ -4210,8 +4735,11 @@
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="168" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
         <v>4</v>
       </c>
@@ -4231,8 +4759,11 @@
       <c r="O168">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q168">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B169" t="s">
         <v>4</v>
       </c>
@@ -4252,8 +4783,11 @@
       <c r="O169">
         <v>4</v>
       </c>
-    </row>
-    <row r="170" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q169">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
         <v>4</v>
       </c>
@@ -4276,8 +4810,11 @@
       <c r="O170">
         <v>7</v>
       </c>
-    </row>
-    <row r="171" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q170">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
         <v>3</v>
       </c>
@@ -4294,8 +4831,11 @@
       <c r="O171">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
         <v>3</v>
       </c>
@@ -4315,8 +4855,11 @@
       <c r="O172">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q172">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
         <v>3</v>
       </c>
@@ -4336,8 +4879,11 @@
       <c r="O173">
         <v>5</v>
       </c>
-    </row>
-    <row r="174" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q173">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B174" t="s">
         <v>3</v>
       </c>
@@ -4360,8 +4906,11 @@
       <c r="O174">
         <v>6</v>
       </c>
-    </row>
-    <row r="175" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q174">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
         <v>1</v>
       </c>
@@ -4375,8 +4924,11 @@
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="176" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
         <v>1</v>
       </c>
@@ -4390,8 +4942,11 @@
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="177" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
         <v>1</v>
       </c>
@@ -4411,8 +4966,11 @@
       <c r="O177">
         <v>3</v>
       </c>
-    </row>
-    <row r="178" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
         <v>1</v>
       </c>
@@ -4438,8 +4996,11 @@
       <c r="O178">
         <v>4</v>
       </c>
-    </row>
-    <row r="179" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B179" t="s">
         <v>4</v>
       </c>
@@ -4453,8 +5014,11 @@
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="180" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B180" t="s">
         <v>4</v>
       </c>
@@ -4474,8 +5038,11 @@
       <c r="O180">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
         <v>4</v>
       </c>
@@ -4495,8 +5062,11 @@
       <c r="O181">
         <v>7</v>
       </c>
-    </row>
-    <row r="182" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q181">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
         <v>4</v>
       </c>
@@ -4519,8 +5089,11 @@
       <c r="O182">
         <v>6</v>
       </c>
-    </row>
-    <row r="183" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q182">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
         <v>3</v>
       </c>
@@ -4536,8 +5109,11 @@
       <c r="O183">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
         <v>1</v>
       </c>
@@ -4556,8 +5132,11 @@
       <c r="O184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
         <v>3</v>
       </c>
@@ -4576,8 +5155,11 @@
       <c r="O185">
         <v>4</v>
       </c>
-    </row>
-    <row r="186" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q185">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
         <v>1</v>
       </c>
@@ -4596,8 +5178,11 @@
       <c r="O186">
         <v>3</v>
       </c>
-    </row>
-    <row r="187" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q186">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
         <v>4</v>
       </c>
@@ -4613,8 +5198,11 @@
       <c r="O187">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q187">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
         <v>4</v>
       </c>
@@ -4633,8 +5221,11 @@
       <c r="O188">
         <v>6</v>
       </c>
-    </row>
-    <row r="189" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q188">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
         <v>3</v>
       </c>
@@ -4650,8 +5241,11 @@
       <c r="O189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
         <v>1</v>
       </c>
@@ -4670,8 +5264,11 @@
       <c r="O190">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q190">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
         <v>3</v>
       </c>
@@ -4693,8 +5290,11 @@
       <c r="O191">
         <v>5</v>
       </c>
-    </row>
-    <row r="192" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q191">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
         <v>1</v>
       </c>
@@ -4713,8 +5313,11 @@
       <c r="O192">
         <v>2</v>
       </c>
-    </row>
-    <row r="193" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B193" t="s">
         <v>4</v>
       </c>
@@ -4730,8 +5333,11 @@
       <c r="O193">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B194" t="s">
         <v>4</v>
       </c>
@@ -4753,8 +5359,11 @@
       <c r="O194">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q194">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B195" t="s">
         <v>3</v>
       </c>
@@ -4770,8 +5379,11 @@
       <c r="O195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B196" t="s">
         <v>1</v>
       </c>
@@ -4793,8 +5405,11 @@
       <c r="O196">
         <v>4</v>
       </c>
-    </row>
-    <row r="197" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q196">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B197" t="s">
         <v>3</v>
       </c>
@@ -4813,8 +5428,11 @@
       <c r="O197">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B198" t="s">
         <v>1</v>
       </c>
@@ -4833,8 +5451,11 @@
       <c r="O198">
         <v>4</v>
       </c>
-    </row>
-    <row r="199" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B199" t="s">
         <v>4</v>
       </c>
@@ -4850,8 +5471,11 @@
       <c r="O199">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B200" t="s">
         <v>4</v>
       </c>
@@ -4873,8 +5497,11 @@
       <c r="O200">
         <v>5</v>
       </c>
-    </row>
-    <row r="201" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q200">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B201" t="s">
         <v>3</v>
       </c>
@@ -4890,8 +5517,11 @@
       <c r="O201">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B202" t="s">
         <v>1</v>
       </c>
@@ -4910,8 +5540,11 @@
       <c r="O202">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q202">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B203" t="s">
         <v>3</v>
       </c>
@@ -4930,8 +5563,11 @@
       <c r="O203">
         <v>5</v>
       </c>
-    </row>
-    <row r="204" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q203">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B204" t="s">
         <v>1</v>
       </c>
@@ -4950,8 +5586,11 @@
       <c r="O204">
         <v>3</v>
       </c>
-    </row>
-    <row r="205" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B205" t="s">
         <v>4</v>
       </c>
@@ -4967,8 +5606,11 @@
       <c r="O205">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
         <v>4</v>
       </c>
@@ -4987,8 +5629,11 @@
       <c r="O206">
         <v>4</v>
       </c>
-    </row>
-    <row r="207" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q206">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
         <v>3</v>
       </c>
@@ -5004,8 +5649,11 @@
       <c r="O207">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B208" t="s">
         <v>1</v>
       </c>
@@ -5024,8 +5672,11 @@
       <c r="O208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q208">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B209" t="s">
         <v>3</v>
       </c>
@@ -5044,8 +5695,11 @@
       <c r="O209">
         <v>4</v>
       </c>
-    </row>
-    <row r="210" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q209">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B210" t="s">
         <v>1</v>
       </c>
@@ -5064,8 +5718,11 @@
       <c r="O210">
         <v>5</v>
       </c>
-    </row>
-    <row r="211" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q210">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B211" t="s">
         <v>4</v>
       </c>
@@ -5081,8 +5738,11 @@
       <c r="O211">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B212" t="s">
         <v>4</v>
       </c>
@@ -5101,13 +5761,16 @@
       <c r="O212">
         <v>3</v>
       </c>
-    </row>
-    <row r="213" spans="2:15" hidden="1" x14ac:dyDescent="0.2"/>
+      <c r="Q212">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data collection on DOY 351
</commit_message>
<xml_diff>
--- a/data/germination_data.xlsx
+++ b/data/germination_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanmeier/git/morasoilinoculation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\morasoilinoculation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A0342E-3429-CD41-A965-980DFEB39417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E72474-8722-4AE6-A3CF-B637CA5E8092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="680" windowWidth="24980" windowHeight="17240" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="63">
   <si>
     <t>seed_species</t>
   </si>
@@ -222,6 +222,14 @@
   <si>
     <t>346_dead</t>
   </si>
+  <si>
+    <t>351_alive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>351_dead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -231,20 +239,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -308,11 +316,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AJ213" totalsRowShown="0">
-  <autoFilter ref="B2:AJ213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AL213" totalsRowShown="0">
+  <autoFilter ref="B2:AL213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
     <filterColumn colId="0">
       <filters>
-        <filter val="TSHE"/>
+        <filter val="THPL"/>
       </filters>
     </filterColumn>
     <filterColumn colId="1">
@@ -322,11 +330,11 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="0"/>
+        <filter val="10"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="35">
+  <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{1199D7AD-452C-9D4F-9453-306631F01BCC}" name="soil_species"/>
     <tableColumn id="2" xr3:uid="{11F49906-5A0D-4E4F-BA5C-F91CB62A2174}" name="seed_species"/>
     <tableColumn id="3" xr3:uid="{B695F4B4-8561-9D48-9FF3-12A40CB2B7C7}" name="inoculated_%"/>
@@ -362,6 +370,8 @@
     <tableColumn id="33" xr3:uid="{ACEF41BE-89B0-5A4A-B6F5-0CCC540F81A1}" name="342_dead"/>
     <tableColumn id="34" xr3:uid="{203A86FF-9E5C-384E-AC11-B6CFB0054DB3}" name="346_alive"/>
     <tableColumn id="35" xr3:uid="{DA827A40-0005-6749-8CFC-10F8ED8DF6F0}" name="346_dead"/>
+    <tableColumn id="36" xr3:uid="{FD8B1013-17A7-4553-A22E-DA149A479E2B}" name="351_alive"/>
+    <tableColumn id="37" xr3:uid="{4E0CF983-5E89-48E7-8FEE-EC7F374187C4}" name="351_dead"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -684,20 +694,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68F8197-A530-A948-B005-AEDF71CF4B66}">
-  <dimension ref="B2:AJ213"/>
+  <dimension ref="B2:AL213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="AI214" sqref="AI214"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="73" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="AL179" sqref="AL179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.15234375" customWidth="1"/>
+    <col min="4" max="4" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -803,8 +813,14 @@
       <c r="AJ2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -877,8 +893,14 @@
       <c r="AJ3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK3">
+        <v>3</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -927,8 +949,11 @@
       <c r="AI4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1001,8 +1026,14 @@
       <c r="AJ5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK5">
+        <v>6</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1054,8 +1085,11 @@
       <c r="AI6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -1101,8 +1135,11 @@
       <c r="AI7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -1169,8 +1206,14 @@
       <c r="AJ8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK8">
+        <v>6</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1243,8 +1286,14 @@
       <c r="AJ9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK9">
+        <v>6</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1299,8 +1348,11 @@
       <c r="AI10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1367,8 +1419,14 @@
       <c r="AJ11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK11">
+        <v>6</v>
+      </c>
+      <c r="AL11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -1444,8 +1502,14 @@
       <c r="AJ12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK12">
+        <v>5</v>
+      </c>
+      <c r="AL12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1497,8 +1561,11 @@
       <c r="AI13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -1571,8 +1638,11 @@
       <c r="AI14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1622,8 +1692,14 @@
       <c r="AI15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK15">
+        <v>7</v>
+      </c>
+      <c r="AL15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1688,8 +1764,11 @@
       <c r="AI16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1751,8 +1830,14 @@
       <c r="AJ17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK17">
+        <v>7</v>
+      </c>
+      <c r="AL17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -1799,8 +1884,11 @@
       <c r="AI18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -1862,8 +1950,14 @@
       <c r="AJ19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK19">
+        <v>4</v>
+      </c>
+      <c r="AL19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -1907,8 +2001,11 @@
       <c r="AI20">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -1957,8 +2054,11 @@
       <c r="AI21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -2011,8 +2111,11 @@
       <c r="AI22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -2059,8 +2162,11 @@
       <c r="AI23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -2110,8 +2216,11 @@
       <c r="AI24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -2161,8 +2270,11 @@
       <c r="AI25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -2257,8 +2369,14 @@
       <c r="AJ26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK26">
+        <v>6</v>
+      </c>
+      <c r="AL26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -2308,8 +2426,11 @@
       <c r="AI27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -2383,8 +2504,14 @@
       <c r="AJ28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK28">
+        <v>8</v>
+      </c>
+      <c r="AL28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -2434,8 +2561,11 @@
       <c r="AI29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -2491,8 +2621,11 @@
       <c r="AI30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -2563,8 +2696,14 @@
       <c r="AJ31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK31">
+        <v>4</v>
+      </c>
+      <c r="AL31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -2608,8 +2747,11 @@
       <c r="AI32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -2662,8 +2804,11 @@
       <c r="AI33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -2740,8 +2885,14 @@
       <c r="AJ34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK34">
+        <v>5</v>
+      </c>
+      <c r="AL34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -2788,8 +2939,14 @@
       <c r="AI35">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK35">
+        <v>5</v>
+      </c>
+      <c r="AL35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -2854,8 +3011,14 @@
       <c r="AI36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK36">
+        <v>7</v>
+      </c>
+      <c r="AL36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -2905,8 +3068,11 @@
       <c r="AI37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>4</v>
       </c>
@@ -2995,8 +3161,14 @@
       <c r="AJ38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK38">
+        <v>4</v>
+      </c>
+      <c r="AL38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3067,8 +3239,14 @@
       <c r="AJ39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK39">
+        <v>2</v>
+      </c>
+      <c r="AL39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -3148,8 +3326,14 @@
       <c r="AJ40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK40">
+        <v>5</v>
+      </c>
+      <c r="AL40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -3199,8 +3383,14 @@
       <c r="AI41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK41">
+        <v>5</v>
+      </c>
+      <c r="AL41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -3259,8 +3449,11 @@
       <c r="AI42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>1</v>
       </c>
@@ -3328,8 +3521,14 @@
       <c r="AJ43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK43">
+        <v>7</v>
+      </c>
+      <c r="AL43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>1</v>
       </c>
@@ -3373,8 +3572,11 @@
       <c r="AI44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -3469,8 +3671,14 @@
       <c r="AJ45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK45">
+        <v>6</v>
+      </c>
+      <c r="AL45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>1</v>
       </c>
@@ -3526,8 +3734,11 @@
       <c r="AI46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -3574,8 +3785,11 @@
       <c r="AI47">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>4</v>
       </c>
@@ -3655,8 +3869,14 @@
       <c r="AJ48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK48">
+        <v>7</v>
+      </c>
+      <c r="AL48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -3706,8 +3926,11 @@
       <c r="AI49">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -3802,8 +4025,14 @@
       <c r="AJ50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK50">
+        <v>7</v>
+      </c>
+      <c r="AL50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -3868,8 +4097,14 @@
       <c r="AJ51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK51">
+        <v>4</v>
+      </c>
+      <c r="AL51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -3919,8 +4154,11 @@
       <c r="AI52">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -3979,8 +4217,14 @@
       <c r="AJ53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK53">
+        <v>2</v>
+      </c>
+      <c r="AL53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -4033,8 +4277,11 @@
       <c r="AI54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>1</v>
       </c>
@@ -4087,8 +4334,14 @@
       <c r="AJ55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK55">
+        <v>4</v>
+      </c>
+      <c r="AL55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>1</v>
       </c>
@@ -4132,8 +4385,11 @@
       <c r="AI56">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -4183,8 +4439,11 @@
       <c r="AI57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>1</v>
       </c>
@@ -4240,8 +4499,11 @@
       <c r="AI58">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>4</v>
       </c>
@@ -4288,8 +4550,11 @@
       <c r="AI59">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>4</v>
       </c>
@@ -4342,8 +4607,14 @@
       <c r="AJ60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK60">
+        <v>8</v>
+      </c>
+      <c r="AL60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>4</v>
       </c>
@@ -4393,8 +4664,11 @@
       <c r="AI61">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>4</v>
       </c>
@@ -4477,8 +4751,14 @@
       <c r="AI62">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK62">
+        <v>3</v>
+      </c>
+      <c r="AL62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>3</v>
       </c>
@@ -4540,8 +4820,14 @@
       <c r="AJ63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK63">
+        <v>6</v>
+      </c>
+      <c r="AL63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>3</v>
       </c>
@@ -4594,8 +4880,11 @@
       <c r="AI64">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -4645,8 +4934,11 @@
       <c r="AI65">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>3</v>
       </c>
@@ -4696,8 +4988,11 @@
       <c r="AI66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -4768,8 +5063,14 @@
       <c r="AJ67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK67">
+        <v>9</v>
+      </c>
+      <c r="AL67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -4813,8 +5114,11 @@
       <c r="AI68">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK68">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>1</v>
       </c>
@@ -4864,8 +5168,11 @@
       <c r="AI69">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>1</v>
       </c>
@@ -4924,8 +5231,11 @@
       <c r="AI70">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>4</v>
       </c>
@@ -4972,8 +5282,14 @@
       <c r="AI71">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK71">
+        <v>9</v>
+      </c>
+      <c r="AL71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>4</v>
       </c>
@@ -5035,8 +5351,14 @@
       <c r="AJ72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK72">
+        <v>6</v>
+      </c>
+      <c r="AL72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>4</v>
       </c>
@@ -5086,8 +5408,14 @@
       <c r="AI73">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK73">
+        <v>7</v>
+      </c>
+      <c r="AL73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>4</v>
       </c>
@@ -5146,8 +5474,11 @@
       <c r="AI74">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>3</v>
       </c>
@@ -5197,8 +5528,14 @@
       <c r="AI75">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK75">
+        <v>6</v>
+      </c>
+      <c r="AL75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>3</v>
       </c>
@@ -5275,8 +5612,14 @@
       <c r="AJ76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK76">
+        <v>7</v>
+      </c>
+      <c r="AL76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>3</v>
       </c>
@@ -5329,8 +5672,11 @@
       <c r="AI77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK77">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>3</v>
       </c>
@@ -5383,8 +5729,11 @@
       <c r="AI78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>1</v>
       </c>
@@ -5458,8 +5807,14 @@
       <c r="AJ79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK79">
+        <v>7</v>
+      </c>
+      <c r="AL79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>1</v>
       </c>
@@ -5503,8 +5858,14 @@
       <c r="AI80">
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK80">
+        <v>9</v>
+      </c>
+      <c r="AL80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>1</v>
       </c>
@@ -5560,8 +5921,14 @@
       <c r="AI81">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK81">
+        <v>5</v>
+      </c>
+      <c r="AL81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>1</v>
       </c>
@@ -5638,8 +6005,14 @@
       <c r="AJ82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK82">
+        <v>6</v>
+      </c>
+      <c r="AL82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>4</v>
       </c>
@@ -5713,8 +6086,14 @@
       <c r="AJ83">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK83">
+        <v>5</v>
+      </c>
+      <c r="AL83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>4</v>
       </c>
@@ -5788,8 +6167,14 @@
       <c r="AJ84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK84">
+        <v>7</v>
+      </c>
+      <c r="AL84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>4</v>
       </c>
@@ -5857,8 +6242,14 @@
       <c r="AJ85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK85">
+        <v>4</v>
+      </c>
+      <c r="AL85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>4</v>
       </c>
@@ -5917,8 +6308,11 @@
       <c r="AI86">
         <v>8</v>
       </c>
-    </row>
-    <row r="87" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK86">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>3</v>
       </c>
@@ -5995,8 +6389,14 @@
       <c r="AJ87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK87">
+        <v>5</v>
+      </c>
+      <c r="AL87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>3</v>
       </c>
@@ -6055,8 +6455,14 @@
       <c r="AJ88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK88">
+        <v>5</v>
+      </c>
+      <c r="AL88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>3</v>
       </c>
@@ -6109,8 +6515,11 @@
       <c r="AI89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>3</v>
       </c>
@@ -6163,8 +6572,11 @@
       <c r="AI90">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK90">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>1</v>
       </c>
@@ -6235,8 +6647,14 @@
       <c r="AJ91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK91">
+        <v>5</v>
+      </c>
+      <c r="AL91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>1</v>
       </c>
@@ -6286,8 +6704,14 @@
       <c r="AJ92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK92">
+        <v>5</v>
+      </c>
+      <c r="AL92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>1</v>
       </c>
@@ -6340,8 +6764,11 @@
       <c r="AI93">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>1</v>
       </c>
@@ -6397,8 +6824,11 @@
       <c r="AI94">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>4</v>
       </c>
@@ -6445,8 +6875,11 @@
       <c r="AI95">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>4</v>
       </c>
@@ -6502,8 +6935,14 @@
       <c r="AI96">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK96">
+        <v>8</v>
+      </c>
+      <c r="AL96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>4</v>
       </c>
@@ -6556,8 +6995,11 @@
       <c r="AI97">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>4</v>
       </c>
@@ -6622,8 +7064,14 @@
       <c r="AI98">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK98">
+        <v>4</v>
+      </c>
+      <c r="AL98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>3</v>
       </c>
@@ -6670,8 +7118,11 @@
       <c r="AI99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>3</v>
       </c>
@@ -6721,8 +7172,11 @@
       <c r="AI100">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>3</v>
       </c>
@@ -6772,8 +7226,11 @@
       <c r="AI101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>3</v>
       </c>
@@ -6826,8 +7283,11 @@
       <c r="AI102">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>1</v>
       </c>
@@ -6889,8 +7349,14 @@
       <c r="AJ103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK103">
+        <v>4</v>
+      </c>
+      <c r="AL103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>1</v>
       </c>
@@ -6934,8 +7400,11 @@
       <c r="AI104">
         <v>8</v>
       </c>
-    </row>
-    <row r="105" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>1</v>
       </c>
@@ -6985,8 +7454,14 @@
       <c r="AI105">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK105">
+        <v>4</v>
+      </c>
+      <c r="AL105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>1</v>
       </c>
@@ -7057,8 +7532,14 @@
       <c r="AJ106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK106">
+        <v>5</v>
+      </c>
+      <c r="AL106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>4</v>
       </c>
@@ -7120,8 +7601,14 @@
       <c r="AJ107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK107">
+        <v>4</v>
+      </c>
+      <c r="AL107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>4</v>
       </c>
@@ -7168,8 +7655,11 @@
       <c r="AI108">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>4</v>
       </c>
@@ -7219,8 +7709,14 @@
       <c r="AI109">
         <v>9</v>
       </c>
-    </row>
-    <row r="110" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK109">
+        <v>7</v>
+      </c>
+      <c r="AL109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>4</v>
       </c>
@@ -7288,8 +7784,11 @@
       <c r="AI110">
         <v>7</v>
       </c>
-    </row>
-    <row r="111" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK110">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>3</v>
       </c>
@@ -7342,8 +7841,11 @@
       <c r="AI111">
         <v>6</v>
       </c>
-    </row>
-    <row r="112" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK111">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>3</v>
       </c>
@@ -7399,8 +7901,14 @@
       <c r="AJ112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK112">
+        <v>7</v>
+      </c>
+      <c r="AL112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>3</v>
       </c>
@@ -7471,8 +7979,11 @@
       <c r="AJ113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK113">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>3</v>
       </c>
@@ -7525,8 +8036,14 @@
       <c r="AI114">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK114">
+        <v>6</v>
+      </c>
+      <c r="AL114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>1</v>
       </c>
@@ -7600,8 +8117,14 @@
       <c r="AJ115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK115">
+        <v>2</v>
+      </c>
+      <c r="AL115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>1</v>
       </c>
@@ -7645,8 +8168,11 @@
       <c r="AI116">
         <v>7</v>
       </c>
-    </row>
-    <row r="117" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK116">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>1</v>
       </c>
@@ -7696,8 +8222,14 @@
       <c r="AI117">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK117">
+        <v>3</v>
+      </c>
+      <c r="AL117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>1</v>
       </c>
@@ -7754,8 +8286,11 @@
       <c r="AI118">
         <v>6</v>
       </c>
-    </row>
-    <row r="119" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>4</v>
       </c>
@@ -7802,8 +8337,11 @@
       <c r="AI119">
         <v>7</v>
       </c>
-    </row>
-    <row r="120" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK119">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>4</v>
       </c>
@@ -7853,8 +8391,11 @@
       <c r="AI120">
         <v>10</v>
       </c>
-    </row>
-    <row r="121" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK120">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>4</v>
       </c>
@@ -7904,8 +8445,11 @@
       <c r="AI121">
         <v>7</v>
       </c>
-    </row>
-    <row r="122" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK121">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>4</v>
       </c>
@@ -7961,8 +8505,11 @@
       <c r="AI122">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -8015,8 +8562,14 @@
       <c r="AJ123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK123">
+        <v>4</v>
+      </c>
+      <c r="AL123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>3</v>
       </c>
@@ -8096,8 +8649,14 @@
       <c r="AJ124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK124">
+        <v>7</v>
+      </c>
+      <c r="AL124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>3</v>
       </c>
@@ -8177,8 +8736,14 @@
       <c r="AJ125">
         <v>5</v>
       </c>
-    </row>
-    <row r="126" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK125">
+        <v>0</v>
+      </c>
+      <c r="AL125">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>3</v>
       </c>
@@ -8237,8 +8802,14 @@
       <c r="AJ126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK126">
+        <v>5</v>
+      </c>
+      <c r="AL126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>1</v>
       </c>
@@ -8294,8 +8865,14 @@
       <c r="AJ127">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK127">
+        <v>2</v>
+      </c>
+      <c r="AL127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>1</v>
       </c>
@@ -8339,8 +8916,11 @@
       <c r="AI128">
         <v>6</v>
       </c>
-    </row>
-    <row r="129" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK128">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>1</v>
       </c>
@@ -8396,8 +8976,14 @@
       <c r="AI129">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK129">
+        <v>4</v>
+      </c>
+      <c r="AL129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>1</v>
       </c>
@@ -8453,8 +9039,11 @@
       <c r="AI130">
         <v>6</v>
       </c>
-    </row>
-    <row r="131" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK130">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>4</v>
       </c>
@@ -8498,8 +9087,14 @@
       <c r="AI131">
         <v>7</v>
       </c>
-    </row>
-    <row r="132" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK131">
+        <v>6</v>
+      </c>
+      <c r="AL131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>4</v>
       </c>
@@ -8546,8 +9141,11 @@
       <c r="AI132">
         <v>6</v>
       </c>
-    </row>
-    <row r="133" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>4</v>
       </c>
@@ -8597,8 +9195,14 @@
       <c r="AI133">
         <v>6</v>
       </c>
-    </row>
-    <row r="134" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK133">
+        <v>5</v>
+      </c>
+      <c r="AL133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
         <v>4</v>
       </c>
@@ -8657,8 +9261,11 @@
       <c r="AI134">
         <v>10</v>
       </c>
-    </row>
-    <row r="135" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK134">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
         <v>3</v>
       </c>
@@ -8708,8 +9315,11 @@
       <c r="AI135">
         <v>7</v>
       </c>
-    </row>
-    <row r="136" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK135">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
         <v>3</v>
       </c>
@@ -8759,8 +9369,11 @@
       <c r="AI136">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK136">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
         <v>3</v>
       </c>
@@ -8813,8 +9426,14 @@
       <c r="AI137">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK137">
+        <v>4</v>
+      </c>
+      <c r="AL137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
         <v>3</v>
       </c>
@@ -8876,8 +9495,14 @@
       <c r="AJ138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK138">
+        <v>7</v>
+      </c>
+      <c r="AL138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
         <v>1</v>
       </c>
@@ -8921,8 +9546,14 @@
       <c r="AI139">
         <v>6</v>
       </c>
-    </row>
-    <row r="140" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK139">
+        <v>5</v>
+      </c>
+      <c r="AL139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
         <v>1</v>
       </c>
@@ -8966,8 +9597,11 @@
       <c r="AI140">
         <v>8</v>
       </c>
-    </row>
-    <row r="141" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK140">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
         <v>1</v>
       </c>
@@ -9050,8 +9684,14 @@
       <c r="AJ141">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK141">
+        <v>4</v>
+      </c>
+      <c r="AL141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>1</v>
       </c>
@@ -9131,8 +9771,14 @@
       <c r="AJ142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK142">
+        <v>6</v>
+      </c>
+      <c r="AL142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>4</v>
       </c>
@@ -9176,8 +9822,11 @@
       <c r="AI143">
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK143">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>4</v>
       </c>
@@ -9224,8 +9873,11 @@
       <c r="AI144">
         <v>7</v>
       </c>
-    </row>
-    <row r="145" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK144">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>4</v>
       </c>
@@ -9278,8 +9930,11 @@
       <c r="AI145">
         <v>7</v>
       </c>
-    </row>
-    <row r="146" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK145">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>4</v>
       </c>
@@ -9350,8 +10005,14 @@
       <c r="AI146">
         <v>9</v>
       </c>
-    </row>
-    <row r="147" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK146">
+        <v>8</v>
+      </c>
+      <c r="AL146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>3</v>
       </c>
@@ -9413,8 +10074,14 @@
       <c r="AJ147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK147">
+        <v>1</v>
+      </c>
+      <c r="AL147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>3</v>
       </c>
@@ -9464,8 +10131,11 @@
       <c r="AI148">
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>3</v>
       </c>
@@ -9521,8 +10191,14 @@
       <c r="AJ149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK149">
+        <v>3</v>
+      </c>
+      <c r="AL149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>3</v>
       </c>
@@ -9599,8 +10275,14 @@
       <c r="AJ150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK150">
+        <v>8</v>
+      </c>
+      <c r="AL150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
         <v>1</v>
       </c>
@@ -9644,8 +10326,11 @@
       <c r="AI151">
         <v>7</v>
       </c>
-    </row>
-    <row r="152" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
         <v>1</v>
       </c>
@@ -9689,8 +10374,11 @@
       <c r="AI152">
         <v>9</v>
       </c>
-    </row>
-    <row r="153" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK152">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
         <v>1</v>
       </c>
@@ -9740,8 +10428,14 @@
       <c r="AI153">
         <v>6</v>
       </c>
-    </row>
-    <row r="154" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK153">
+        <v>5</v>
+      </c>
+      <c r="AL153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
         <v>1</v>
       </c>
@@ -9827,8 +10521,14 @@
       <c r="AJ154">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK154">
+        <v>4</v>
+      </c>
+      <c r="AL154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
         <v>4</v>
       </c>
@@ -9881,8 +10581,14 @@
       <c r="AJ155">
         <v>2</v>
       </c>
-    </row>
-    <row r="156" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK155">
+        <v>7</v>
+      </c>
+      <c r="AL155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
         <v>4</v>
       </c>
@@ -9932,8 +10638,11 @@
       <c r="AI156">
         <v>6</v>
       </c>
-    </row>
-    <row r="157" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK156">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
         <v>4</v>
       </c>
@@ -9983,8 +10692,14 @@
       <c r="AI157">
         <v>5</v>
       </c>
-    </row>
-    <row r="158" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK157">
+        <v>4</v>
+      </c>
+      <c r="AL157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B158" t="s">
         <v>4</v>
       </c>
@@ -10043,8 +10758,11 @@
       <c r="AI158">
         <v>7</v>
       </c>
-    </row>
-    <row r="159" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK158">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B159" t="s">
         <v>3</v>
       </c>
@@ -10097,8 +10815,14 @@
       <c r="AJ159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK159">
+        <v>4</v>
+      </c>
+      <c r="AL159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B160" t="s">
         <v>3</v>
       </c>
@@ -10148,8 +10872,11 @@
       <c r="AI160">
         <v>9</v>
       </c>
-    </row>
-    <row r="161" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK160">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B161" t="s">
         <v>3</v>
       </c>
@@ -10226,8 +10953,14 @@
       <c r="AJ161">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK161">
+        <v>2</v>
+      </c>
+      <c r="AL161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
         <v>3</v>
       </c>
@@ -10280,8 +11013,11 @@
       <c r="AI162">
         <v>8</v>
       </c>
-    </row>
-    <row r="163" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK162">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>1</v>
       </c>
@@ -10331,8 +11067,14 @@
       <c r="AJ163">
         <v>2</v>
       </c>
-    </row>
-    <row r="164" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK163">
+        <v>4</v>
+      </c>
+      <c r="AL163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>1</v>
       </c>
@@ -10376,8 +11118,11 @@
       <c r="AI164">
         <v>9</v>
       </c>
-    </row>
-    <row r="165" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK164">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>1</v>
       </c>
@@ -10427,8 +11172,14 @@
       <c r="AI165">
         <v>5</v>
       </c>
-    </row>
-    <row r="166" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK165">
+        <v>4</v>
+      </c>
+      <c r="AL165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>1</v>
       </c>
@@ -10499,8 +11250,14 @@
       <c r="AJ166">
         <v>2</v>
       </c>
-    </row>
-    <row r="167" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK166">
+        <v>3</v>
+      </c>
+      <c r="AL166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
         <v>4</v>
       </c>
@@ -10544,8 +11301,11 @@
       <c r="AI167">
         <v>7</v>
       </c>
-    </row>
-    <row r="168" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK167">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
         <v>4</v>
       </c>
@@ -10601,8 +11361,14 @@
       <c r="AI168">
         <v>10</v>
       </c>
-    </row>
-    <row r="169" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK168">
+        <v>9</v>
+      </c>
+      <c r="AL168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B169" t="s">
         <v>4</v>
       </c>
@@ -10652,8 +11418,11 @@
       <c r="AI169">
         <v>6</v>
       </c>
-    </row>
-    <row r="170" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK169">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
         <v>4</v>
       </c>
@@ -10706,8 +11475,11 @@
       <c r="AI170">
         <v>7</v>
       </c>
-    </row>
-    <row r="171" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK170">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
         <v>3</v>
       </c>
@@ -10766,8 +11538,14 @@
       <c r="AJ171">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK171">
+        <v>5</v>
+      </c>
+      <c r="AL171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
         <v>3</v>
       </c>
@@ -10817,8 +11595,11 @@
       <c r="AI172">
         <v>8</v>
       </c>
-    </row>
-    <row r="173" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK172">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
         <v>3</v>
       </c>
@@ -10868,8 +11649,11 @@
       <c r="AI173">
         <v>6</v>
       </c>
-    </row>
-    <row r="174" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK173">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B174" t="s">
         <v>3</v>
       </c>
@@ -10922,8 +11706,11 @@
       <c r="AI174">
         <v>9</v>
       </c>
-    </row>
-    <row r="175" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK174">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
         <v>1</v>
       </c>
@@ -10973,8 +11760,14 @@
       <c r="AJ175">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK175">
+        <v>8</v>
+      </c>
+      <c r="AL175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
         <v>1</v>
       </c>
@@ -11018,8 +11811,11 @@
       <c r="AI176">
         <v>8</v>
       </c>
-    </row>
-    <row r="177" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK176">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
         <v>1</v>
       </c>
@@ -11069,8 +11865,11 @@
       <c r="AI177">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
         <v>1</v>
       </c>
@@ -11126,8 +11925,11 @@
       <c r="AI178">
         <v>6</v>
       </c>
-    </row>
-    <row r="179" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK178">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="2:38" x14ac:dyDescent="0.35">
       <c r="B179" t="s">
         <v>4</v>
       </c>
@@ -11180,8 +11982,14 @@
       <c r="AJ179">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK179">
+        <v>7</v>
+      </c>
+      <c r="AL179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B180" t="s">
         <v>4</v>
       </c>
@@ -11231,8 +12039,11 @@
       <c r="AI180">
         <v>8</v>
       </c>
-    </row>
-    <row r="181" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK180">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
         <v>4</v>
       </c>
@@ -11282,8 +12093,14 @@
       <c r="AI181">
         <v>7</v>
       </c>
-    </row>
-    <row r="182" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK181">
+        <v>5</v>
+      </c>
+      <c r="AL181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
         <v>4</v>
       </c>
@@ -11336,8 +12153,11 @@
       <c r="AI182">
         <v>6</v>
       </c>
-    </row>
-    <row r="183" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK182">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
         <v>3</v>
       </c>
@@ -11404,8 +12224,14 @@
       <c r="AJ183">
         <v>2</v>
       </c>
-    </row>
-    <row r="184" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK183">
+        <v>5</v>
+      </c>
+      <c r="AL183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
         <v>1</v>
       </c>
@@ -11454,8 +12280,11 @@
       <c r="AI184">
         <v>6</v>
       </c>
-    </row>
-    <row r="185" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK184">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
         <v>3</v>
       </c>
@@ -11504,8 +12333,14 @@
       <c r="AI185">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK185">
+        <v>3</v>
+      </c>
+      <c r="AL185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
         <v>1</v>
       </c>
@@ -11554,8 +12389,11 @@
       <c r="AI186">
         <v>7</v>
       </c>
-    </row>
-    <row r="187" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK186">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
         <v>4</v>
       </c>
@@ -11601,8 +12439,11 @@
       <c r="AI187">
         <v>7</v>
       </c>
-    </row>
-    <row r="188" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK187">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="188" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
         <v>4</v>
       </c>
@@ -11651,8 +12492,14 @@
       <c r="AI188">
         <v>10</v>
       </c>
-    </row>
-    <row r="189" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK188">
+        <v>9</v>
+      </c>
+      <c r="AL188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
         <v>3</v>
       </c>
@@ -11722,8 +12569,14 @@
       <c r="AJ189">
         <v>2</v>
       </c>
-    </row>
-    <row r="190" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK189">
+        <v>2</v>
+      </c>
+      <c r="AL189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
         <v>1</v>
       </c>
@@ -11784,8 +12637,14 @@
       <c r="AJ190">
         <v>2</v>
       </c>
-    </row>
-    <row r="191" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK190">
+        <v>3</v>
+      </c>
+      <c r="AL190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
         <v>3</v>
       </c>
@@ -11846,8 +12705,14 @@
       <c r="AJ191">
         <v>2</v>
       </c>
-    </row>
-    <row r="192" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK191">
+        <v>1</v>
+      </c>
+      <c r="AL191">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
         <v>1</v>
       </c>
@@ -11896,8 +12761,14 @@
       <c r="AI192">
         <v>3</v>
       </c>
-    </row>
-    <row r="193" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK192">
+        <v>1</v>
+      </c>
+      <c r="AL192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B193" t="s">
         <v>4</v>
       </c>
@@ -11967,8 +12838,14 @@
       <c r="AJ193">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK193">
+        <v>6</v>
+      </c>
+      <c r="AL193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B194" t="s">
         <v>4</v>
       </c>
@@ -12020,8 +12897,11 @@
       <c r="AI194">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK194">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B195" t="s">
         <v>3</v>
       </c>
@@ -12088,8 +12968,14 @@
       <c r="AJ195">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK195">
+        <v>2</v>
+      </c>
+      <c r="AL195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B196" t="s">
         <v>1</v>
       </c>
@@ -12162,8 +13048,14 @@
       <c r="AJ196">
         <v>2</v>
       </c>
-    </row>
-    <row r="197" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK196">
+        <v>5</v>
+      </c>
+      <c r="AL196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B197" t="s">
         <v>3</v>
       </c>
@@ -12221,8 +13113,11 @@
       <c r="AI197">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B198" t="s">
         <v>1</v>
       </c>
@@ -12271,8 +13166,11 @@
       <c r="AI198">
         <v>5</v>
       </c>
-    </row>
-    <row r="199" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK198">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B199" t="s">
         <v>4</v>
       </c>
@@ -12327,8 +13225,14 @@
       <c r="AJ199">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK199">
+        <v>5</v>
+      </c>
+      <c r="AL199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B200" t="s">
         <v>4</v>
       </c>
@@ -12380,8 +13284,11 @@
       <c r="AI200">
         <v>7</v>
       </c>
-    </row>
-    <row r="201" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK200">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B201" t="s">
         <v>3</v>
       </c>
@@ -12439,8 +13346,14 @@
       <c r="AJ201">
         <v>2</v>
       </c>
-    </row>
-    <row r="202" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK201">
+        <v>3</v>
+      </c>
+      <c r="AL201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B202" t="s">
         <v>1</v>
       </c>
@@ -12507,8 +13420,14 @@
       <c r="AJ202">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK202">
+        <v>0</v>
+      </c>
+      <c r="AL202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B203" t="s">
         <v>3</v>
       </c>
@@ -12563,8 +13482,14 @@
       <c r="AJ203">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK203">
+        <v>3</v>
+      </c>
+      <c r="AL203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B204" t="s">
         <v>1</v>
       </c>
@@ -12613,8 +13538,11 @@
       <c r="AI204">
         <v>4</v>
       </c>
-    </row>
-    <row r="205" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK204">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B205" t="s">
         <v>4</v>
       </c>
@@ -12687,8 +13615,14 @@
       <c r="AJ205">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK205">
+        <v>9</v>
+      </c>
+      <c r="AL205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
         <v>4</v>
       </c>
@@ -12737,8 +13671,11 @@
       <c r="AI206">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK206">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
         <v>3</v>
       </c>
@@ -12784,8 +13721,11 @@
       <c r="AI207">
         <v>4</v>
       </c>
-    </row>
-    <row r="208" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B208" t="s">
         <v>1</v>
       </c>
@@ -12849,8 +13789,14 @@
       <c r="AJ208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK208">
+        <v>2</v>
+      </c>
+      <c r="AL208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B209" t="s">
         <v>3</v>
       </c>
@@ -12899,8 +13845,14 @@
       <c r="AI209">
         <v>5</v>
       </c>
-    </row>
-    <row r="210" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK209">
+        <v>4</v>
+      </c>
+      <c r="AL209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B210" t="s">
         <v>1</v>
       </c>
@@ -12970,8 +13922,14 @@
       <c r="AJ210">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK210">
+        <v>4</v>
+      </c>
+      <c r="AL210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B211" t="s">
         <v>4</v>
       </c>
@@ -13017,8 +13975,14 @@
       <c r="AI211">
         <v>5</v>
       </c>
-    </row>
-    <row r="212" spans="2:36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AK211">
+        <v>4</v>
+      </c>
+      <c r="AL211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="2:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="B212" t="s">
         <v>4</v>
       </c>
@@ -13067,8 +14031,14 @@
       <c r="AI212">
         <v>5</v>
       </c>
-    </row>
-    <row r="213" spans="2:36" hidden="1" x14ac:dyDescent="0.2"/>
+      <c r="AK212">
+        <v>4</v>
+      </c>
+      <c r="AL212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="2:38" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data collection for the last time in 2025
</commit_message>
<xml_diff>
--- a/data/germination_data.xlsx
+++ b/data/germination_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\morasoilinoculation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DBB32C-43A4-4D03-823A-A9DCF38990C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4C972F-59D2-4E48-B228-A858BA21171B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="71">
   <si>
     <t>seed_species</t>
   </si>
@@ -260,6 +260,14 @@
     <t>doy328: dead germinants very hard to see; doy 358: green moss?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>365_alive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>365_dead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -346,8 +354,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AN213" totalsRowShown="0">
-  <autoFilter ref="B2:AN213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AP213" totalsRowShown="0">
+  <autoFilter ref="B2:AP213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
     <filterColumn colId="0">
       <filters>
         <filter val="THPL"/>
@@ -355,16 +363,16 @@
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="TSHE"/>
+        <filter val="PSME"/>
       </filters>
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="10"/>
+        <filter val="0"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="39">
+  <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{1199D7AD-452C-9D4F-9453-306631F01BCC}" name="soil_species"/>
     <tableColumn id="2" xr3:uid="{11F49906-5A0D-4E4F-BA5C-F91CB62A2174}" name="seed_species"/>
     <tableColumn id="3" xr3:uid="{B695F4B4-8561-9D48-9FF3-12A40CB2B7C7}" name="inoculated_%"/>
@@ -404,6 +412,8 @@
     <tableColumn id="37" xr3:uid="{4E0CF983-5E89-48E7-8FEE-EC7F374187C4}" name="351_dead"/>
     <tableColumn id="38" xr3:uid="{24DFCEB5-9EBF-4889-BF53-BBA7F1ED10C8}" name="358_alive"/>
     <tableColumn id="39" xr3:uid="{26B0383B-95B6-4DD5-B7B4-685313FCC697}" name="358_dead2"/>
+    <tableColumn id="40" xr3:uid="{77E0EA7E-1234-4ADB-9C12-30309866C064}" name="365_alive"/>
+    <tableColumn id="41" xr3:uid="{B72A1CA6-FECC-4A5F-8AE4-79F078A65708}" name="365_dead"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68F8197-A530-A948-B005-AEDF71CF4B66}">
-  <dimension ref="B2:AN213"/>
+  <dimension ref="B2:AP213"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="73" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="AO146" sqref="AO146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -739,7 +749,7 @@
     <col min="4" max="4" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -857,8 +867,14 @@
       <c r="AN2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -943,8 +959,14 @@
       <c r="AN3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO3">
+        <v>3</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1002,8 +1024,11 @@
       <c r="AM4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1088,8 +1113,14 @@
       <c r="AN5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO5">
+        <v>6</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1147,8 +1178,11 @@
       <c r="AM6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -1200,8 +1234,14 @@
       <c r="AM7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO7">
+        <v>5</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -1280,8 +1320,14 @@
       <c r="AN8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO8">
+        <v>6</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1366,8 +1412,14 @@
       <c r="AN9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO9">
+        <v>6</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1428,8 +1480,11 @@
       <c r="AM10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1508,8 +1563,14 @@
       <c r="AN11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO11">
+        <v>6</v>
+      </c>
+      <c r="AP11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -1597,8 +1658,11 @@
       <c r="AN12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1656,8 +1720,14 @@
       <c r="AM13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO13">
+        <v>5</v>
+      </c>
+      <c r="AP13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -1736,8 +1806,11 @@
       <c r="AM14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1802,8 +1875,14 @@
       <c r="AN15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO15">
+        <v>7</v>
+      </c>
+      <c r="AP15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1874,8 +1953,11 @@
       <c r="AM16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1949,8 +2031,14 @@
       <c r="AN17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO17">
+        <v>7</v>
+      </c>
+      <c r="AP17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -2003,8 +2091,11 @@
       <c r="AM18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -2081,8 +2172,14 @@
       <c r="AN19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO19">
+        <v>3</v>
+      </c>
+      <c r="AP19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -2132,8 +2229,14 @@
       <c r="AM20">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO20">
+        <v>13</v>
+      </c>
+      <c r="AP20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -2188,8 +2291,14 @@
       <c r="AM21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO21">
+        <v>5</v>
+      </c>
+      <c r="AP21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -2248,8 +2357,11 @@
       <c r="AM22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -2302,8 +2414,11 @@
       <c r="AM23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -2359,8 +2474,14 @@
       <c r="AM24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO24">
+        <v>9</v>
+      </c>
+      <c r="AP24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -2416,8 +2537,11 @@
       <c r="AM25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -2521,8 +2645,11 @@
       <c r="AM26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -2581,8 +2708,11 @@
       <c r="AM27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -2668,8 +2798,14 @@
       <c r="AN28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO28">
+        <v>7</v>
+      </c>
+      <c r="AP28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -2725,8 +2861,11 @@
       <c r="AM29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -2788,8 +2927,11 @@
       <c r="AM30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -2872,8 +3014,14 @@
       <c r="AN31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO31">
+        <v>4</v>
+      </c>
+      <c r="AP31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -2923,8 +3071,11 @@
       <c r="AM32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -2983,8 +3134,11 @@
       <c r="AM33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -3070,8 +3224,11 @@
       <c r="AM34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -3133,8 +3290,14 @@
       <c r="AN35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO35">
+        <v>6</v>
+      </c>
+      <c r="AP35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -3205,8 +3368,11 @@
       <c r="AM36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -3262,8 +3428,11 @@
       <c r="AM37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>4</v>
       </c>
@@ -3364,8 +3533,14 @@
       <c r="AN38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO38">
+        <v>4</v>
+      </c>
+      <c r="AP38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3448,8 +3623,14 @@
       <c r="AN39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO39">
+        <v>3</v>
+      </c>
+      <c r="AP39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -3544,8 +3725,14 @@
       <c r="AN40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO40">
+        <v>5</v>
+      </c>
+      <c r="AP40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -3607,8 +3794,14 @@
       <c r="AN41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO41">
+        <v>5</v>
+      </c>
+      <c r="AP41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -3673,8 +3866,11 @@
       <c r="AM42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>1</v>
       </c>
@@ -3754,8 +3950,14 @@
       <c r="AN43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO43">
+        <v>7</v>
+      </c>
+      <c r="AP43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>1</v>
       </c>
@@ -3805,8 +4007,11 @@
       <c r="AM44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -3913,8 +4118,14 @@
       <c r="AN45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO45">
+        <v>7</v>
+      </c>
+      <c r="AP45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>1</v>
       </c>
@@ -3976,8 +4187,11 @@
       <c r="AM46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -4033,8 +4247,11 @@
       <c r="AM47">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>4</v>
       </c>
@@ -4126,8 +4343,14 @@
       <c r="AN48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO48">
+        <v>7</v>
+      </c>
+      <c r="AP48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -4183,8 +4406,11 @@
       <c r="AM49">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -4291,8 +4517,14 @@
       <c r="AN50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO50">
+        <v>7</v>
+      </c>
+      <c r="AP50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -4372,8 +4604,14 @@
       <c r="AN51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO51">
+        <v>4</v>
+      </c>
+      <c r="AP51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -4429,8 +4667,11 @@
       <c r="AM52">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -4501,8 +4742,14 @@
       <c r="AN53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO53">
+        <v>2</v>
+      </c>
+      <c r="AP53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -4561,8 +4808,11 @@
       <c r="AM54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>1</v>
       </c>
@@ -4627,8 +4877,14 @@
       <c r="AN55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO55">
+        <v>4</v>
+      </c>
+      <c r="AP55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>1</v>
       </c>
@@ -4678,8 +4934,11 @@
       <c r="AM56">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -4735,8 +4994,11 @@
       <c r="AM57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>1</v>
       </c>
@@ -4798,8 +5060,11 @@
       <c r="AM58">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>4</v>
       </c>
@@ -4852,8 +5117,11 @@
       <c r="AM59">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>4</v>
       </c>
@@ -4918,8 +5186,14 @@
       <c r="AN60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO60">
+        <v>7</v>
+      </c>
+      <c r="AP60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>4</v>
       </c>
@@ -4975,8 +5249,11 @@
       <c r="AM61">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>4</v>
       </c>
@@ -5071,8 +5348,14 @@
       <c r="AN62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO62">
+        <v>3</v>
+      </c>
+      <c r="AP62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>3</v>
       </c>
@@ -5146,8 +5429,14 @@
       <c r="AN63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO63">
+        <v>6</v>
+      </c>
+      <c r="AP63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>3</v>
       </c>
@@ -5206,8 +5495,11 @@
       <c r="AM64">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -5263,8 +5555,11 @@
       <c r="AM65">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>3</v>
       </c>
@@ -5320,8 +5615,11 @@
       <c r="AM66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -5404,8 +5702,14 @@
       <c r="AN67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO67">
+        <v>7</v>
+      </c>
+      <c r="AP67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -5455,8 +5759,11 @@
       <c r="AM68">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO68">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>1</v>
       </c>
@@ -5512,8 +5819,11 @@
       <c r="AM69">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO69">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>1</v>
       </c>
@@ -5578,8 +5888,11 @@
       <c r="AM70">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>4</v>
       </c>
@@ -5641,8 +5954,14 @@
       <c r="AN71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO71">
+        <v>9</v>
+      </c>
+      <c r="AP71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>4</v>
       </c>
@@ -5716,8 +6035,14 @@
       <c r="AN72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO72">
+        <v>6</v>
+      </c>
+      <c r="AP72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>4</v>
       </c>
@@ -5773,8 +6098,11 @@
       <c r="AM73">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>4</v>
       </c>
@@ -5839,8 +6167,11 @@
       <c r="AM74">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>3</v>
       </c>
@@ -5899,8 +6230,14 @@
       <c r="AM75">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO75">
+        <v>6</v>
+      </c>
+      <c r="AP75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>3</v>
       </c>
@@ -5992,8 +6329,14 @@
       <c r="AN76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO76">
+        <v>7</v>
+      </c>
+      <c r="AP76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>3</v>
       </c>
@@ -6052,8 +6395,11 @@
       <c r="AM77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO77">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>3</v>
       </c>
@@ -6112,8 +6458,11 @@
       <c r="AM78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>1</v>
       </c>
@@ -6199,8 +6548,14 @@
       <c r="AN79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO79">
+        <v>7</v>
+      </c>
+      <c r="AP79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>1</v>
       </c>
@@ -6256,8 +6611,14 @@
       <c r="AN80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO80">
+        <v>9</v>
+      </c>
+      <c r="AP80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>1</v>
       </c>
@@ -6325,8 +6686,14 @@
       <c r="AN81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO81">
+        <v>5</v>
+      </c>
+      <c r="AP81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>1</v>
       </c>
@@ -6415,8 +6782,14 @@
       <c r="AN82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO82">
+        <v>7</v>
+      </c>
+      <c r="AP82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>4</v>
       </c>
@@ -6502,8 +6875,14 @@
       <c r="AN83">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO83">
+        <v>5</v>
+      </c>
+      <c r="AP83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>4</v>
       </c>
@@ -6589,8 +6968,14 @@
       <c r="AN84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO84">
+        <v>7</v>
+      </c>
+      <c r="AP84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>4</v>
       </c>
@@ -6673,8 +7058,14 @@
       <c r="AN85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO85">
+        <v>4</v>
+      </c>
+      <c r="AP85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>4</v>
       </c>
@@ -6739,8 +7130,14 @@
       <c r="AM86">
         <v>8</v>
       </c>
-    </row>
-    <row r="87" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO86">
+        <v>7</v>
+      </c>
+      <c r="AP86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>3</v>
       </c>
@@ -6829,8 +7226,14 @@
       <c r="AN87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO87">
+        <v>5</v>
+      </c>
+      <c r="AP87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>3</v>
       </c>
@@ -6904,8 +7307,14 @@
       <c r="AN88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO88">
+        <v>5</v>
+      </c>
+      <c r="AP88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>3</v>
       </c>
@@ -6964,8 +7373,11 @@
       <c r="AM89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>3</v>
       </c>
@@ -7024,8 +7436,11 @@
       <c r="AM90">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO90">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>1</v>
       </c>
@@ -7108,8 +7523,14 @@
       <c r="AN91">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO91">
+        <v>5</v>
+      </c>
+      <c r="AP91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>1</v>
       </c>
@@ -7171,8 +7592,14 @@
       <c r="AN92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO92">
+        <v>5</v>
+      </c>
+      <c r="AP92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>1</v>
       </c>
@@ -7231,8 +7658,11 @@
       <c r="AM93">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>1</v>
       </c>
@@ -7294,8 +7724,11 @@
       <c r="AM94">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>4</v>
       </c>
@@ -7351,8 +7784,11 @@
       <c r="AM95">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>4</v>
       </c>
@@ -7420,8 +7856,14 @@
       <c r="AN96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO96">
+        <v>9</v>
+      </c>
+      <c r="AP96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>4</v>
       </c>
@@ -7480,8 +7922,11 @@
       <c r="AM97">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>4</v>
       </c>
@@ -7552,8 +7997,11 @@
       <c r="AM98">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>3</v>
       </c>
@@ -7606,8 +8054,11 @@
       <c r="AM99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>3</v>
       </c>
@@ -7663,8 +8114,11 @@
       <c r="AM100">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>3</v>
       </c>
@@ -7723,8 +8177,11 @@
       <c r="AM101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>3</v>
       </c>
@@ -7783,8 +8240,11 @@
       <c r="AM102">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>1</v>
       </c>
@@ -7861,8 +8321,14 @@
       <c r="AN103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO103">
+        <v>4</v>
+      </c>
+      <c r="AP103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>1</v>
       </c>
@@ -7912,8 +8378,14 @@
       <c r="AM104">
         <v>8</v>
       </c>
-    </row>
-    <row r="105" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO104">
+        <v>7</v>
+      </c>
+      <c r="AP104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>1</v>
       </c>
@@ -7975,8 +8447,14 @@
       <c r="AN105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO105">
+        <v>4</v>
+      </c>
+      <c r="AP105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>1</v>
       </c>
@@ -8059,8 +8537,14 @@
       <c r="AN106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO106">
+        <v>6</v>
+      </c>
+      <c r="AP106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>4</v>
       </c>
@@ -8134,8 +8618,14 @@
       <c r="AN107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO107">
+        <v>4</v>
+      </c>
+      <c r="AP107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>4</v>
       </c>
@@ -8188,8 +8678,11 @@
       <c r="AM108">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>4</v>
       </c>
@@ -8251,8 +8744,14 @@
       <c r="AN109">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO109">
+        <v>7</v>
+      </c>
+      <c r="AP109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>4</v>
       </c>
@@ -8326,8 +8825,14 @@
       <c r="AM110">
         <v>7</v>
       </c>
-    </row>
-    <row r="111" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO110">
+        <v>6</v>
+      </c>
+      <c r="AP110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>3</v>
       </c>
@@ -8386,8 +8891,11 @@
       <c r="AM111">
         <v>6</v>
       </c>
-    </row>
-    <row r="112" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO111">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>3</v>
       </c>
@@ -8455,8 +8963,14 @@
       <c r="AN112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO112">
+        <v>7</v>
+      </c>
+      <c r="AP112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>3</v>
       </c>
@@ -8539,8 +9053,14 @@
       <c r="AN113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO113">
+        <v>4</v>
+      </c>
+      <c r="AP113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>3</v>
       </c>
@@ -8599,8 +9119,11 @@
       <c r="AM114">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>1</v>
       </c>
@@ -8686,8 +9209,14 @@
       <c r="AN115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO115">
+        <v>2</v>
+      </c>
+      <c r="AP115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>1</v>
       </c>
@@ -8737,8 +9266,14 @@
       <c r="AM116">
         <v>8</v>
       </c>
-    </row>
-    <row r="117" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO116">
+        <v>7</v>
+      </c>
+      <c r="AP116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>1</v>
       </c>
@@ -8800,8 +9335,14 @@
       <c r="AN117">
         <v>2</v>
       </c>
-    </row>
-    <row r="118" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO117">
+        <v>2</v>
+      </c>
+      <c r="AP117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>1</v>
       </c>
@@ -8864,8 +9405,11 @@
       <c r="AM118">
         <v>6</v>
       </c>
-    </row>
-    <row r="119" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>4</v>
       </c>
@@ -8918,8 +9462,11 @@
       <c r="AM119">
         <v>7</v>
       </c>
-    </row>
-    <row r="120" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO119">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>4</v>
       </c>
@@ -8975,8 +9522,11 @@
       <c r="AM120">
         <v>10</v>
       </c>
-    </row>
-    <row r="121" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO120">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>4</v>
       </c>
@@ -9035,8 +9585,11 @@
       <c r="AM121">
         <v>7</v>
       </c>
-    </row>
-    <row r="122" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO121">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>4</v>
       </c>
@@ -9098,8 +9651,11 @@
       <c r="AM122">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -9164,8 +9720,14 @@
       <c r="AN123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO123">
+        <v>4</v>
+      </c>
+      <c r="AP123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>3</v>
       </c>
@@ -9257,8 +9819,14 @@
       <c r="AN124">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO124">
+        <v>7</v>
+      </c>
+      <c r="AP124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>3</v>
       </c>
@@ -9350,8 +9918,14 @@
       <c r="AN125">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO125">
+        <v>0</v>
+      </c>
+      <c r="AP125">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>3</v>
       </c>
@@ -9422,8 +9996,14 @@
       <c r="AN126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO126">
+        <v>5</v>
+      </c>
+      <c r="AP126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>1</v>
       </c>
@@ -9491,8 +10071,14 @@
       <c r="AN127">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO127">
+        <v>2</v>
+      </c>
+      <c r="AP127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>1</v>
       </c>
@@ -9542,8 +10128,11 @@
       <c r="AM128">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO128">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>1</v>
       </c>
@@ -9611,8 +10200,14 @@
       <c r="AN129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO129">
+        <v>4</v>
+      </c>
+      <c r="AP129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>1</v>
       </c>
@@ -9674,8 +10269,11 @@
       <c r="AM130">
         <v>7</v>
       </c>
-    </row>
-    <row r="131" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO130">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>4</v>
       </c>
@@ -9734,8 +10332,14 @@
       <c r="AN131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO131">
+        <v>6</v>
+      </c>
+      <c r="AP131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>4</v>
       </c>
@@ -9788,8 +10392,11 @@
       <c r="AM132">
         <v>6</v>
       </c>
-    </row>
-    <row r="133" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>4</v>
       </c>
@@ -9845,8 +10452,11 @@
       <c r="AM133">
         <v>6</v>
       </c>
-    </row>
-    <row r="134" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
         <v>4</v>
       </c>
@@ -9911,8 +10521,11 @@
       <c r="AM134">
         <v>10</v>
       </c>
-    </row>
-    <row r="135" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO134">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
         <v>3</v>
       </c>
@@ -9968,8 +10581,11 @@
       <c r="AM135">
         <v>7</v>
       </c>
-    </row>
-    <row r="136" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO135">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
         <v>3</v>
       </c>
@@ -10025,8 +10641,11 @@
       <c r="AM136">
         <v>6</v>
       </c>
-    </row>
-    <row r="137" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO136">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
         <v>3</v>
       </c>
@@ -10085,8 +10704,11 @@
       <c r="AM137">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO137">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
         <v>3</v>
       </c>
@@ -10160,8 +10782,14 @@
       <c r="AN138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO138">
+        <v>7</v>
+      </c>
+      <c r="AP138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
         <v>1</v>
       </c>
@@ -10217,8 +10845,14 @@
       <c r="AN139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO139">
+        <v>5</v>
+      </c>
+      <c r="AP139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
         <v>1</v>
       </c>
@@ -10268,8 +10902,11 @@
       <c r="AM140">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO140">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
         <v>1</v>
       </c>
@@ -10364,8 +11001,14 @@
       <c r="AN141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO141">
+        <v>6</v>
+      </c>
+      <c r="AP141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>1</v>
       </c>
@@ -10457,8 +11100,14 @@
       <c r="AN142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO142">
+        <v>6</v>
+      </c>
+      <c r="AP142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>4</v>
       </c>
@@ -10508,8 +11157,11 @@
       <c r="AM143">
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO143">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>4</v>
       </c>
@@ -10562,8 +11214,11 @@
       <c r="AM144">
         <v>7</v>
       </c>
-    </row>
-    <row r="145" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO144">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>4</v>
       </c>
@@ -10622,8 +11277,11 @@
       <c r="AM145">
         <v>7</v>
       </c>
-    </row>
-    <row r="146" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO145">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>4</v>
       </c>
@@ -10706,8 +11364,14 @@
       <c r="AN146">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO146">
+        <v>8</v>
+      </c>
+      <c r="AP146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>3</v>
       </c>
@@ -10784,8 +11448,14 @@
       <c r="AN147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO147">
+        <v>2</v>
+      </c>
+      <c r="AP147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>3</v>
       </c>
@@ -10841,8 +11511,11 @@
       <c r="AM148">
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>3</v>
       </c>
@@ -10910,8 +11583,14 @@
       <c r="AN149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO149">
+        <v>3</v>
+      </c>
+      <c r="AP149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>3</v>
       </c>
@@ -11000,8 +11679,14 @@
       <c r="AN150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO150">
+        <v>8</v>
+      </c>
+      <c r="AP150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
         <v>1</v>
       </c>
@@ -11054,8 +11739,11 @@
       <c r="AM151">
         <v>7</v>
       </c>
-    </row>
-    <row r="152" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
         <v>1</v>
       </c>
@@ -11105,8 +11793,11 @@
       <c r="AM152">
         <v>9</v>
       </c>
-    </row>
-    <row r="153" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO152">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
         <v>1</v>
       </c>
@@ -11168,8 +11859,11 @@
       <c r="AN153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO153">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
         <v>1</v>
       </c>
@@ -11267,8 +11961,14 @@
       <c r="AN154">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO154">
+        <v>4</v>
+      </c>
+      <c r="AP154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
         <v>4</v>
       </c>
@@ -11333,8 +12033,14 @@
       <c r="AN155">
         <v>2</v>
       </c>
-    </row>
-    <row r="156" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO155">
+        <v>6</v>
+      </c>
+      <c r="AP155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
         <v>4</v>
       </c>
@@ -11390,8 +12096,11 @@
       <c r="AM156">
         <v>6</v>
       </c>
-    </row>
-    <row r="157" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO156">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
         <v>4</v>
       </c>
@@ -11450,8 +12159,11 @@
       <c r="AM157">
         <v>5</v>
       </c>
-    </row>
-    <row r="158" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO157">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B158" t="s">
         <v>4</v>
       </c>
@@ -11516,8 +12228,11 @@
       <c r="AM158">
         <v>7</v>
       </c>
-    </row>
-    <row r="159" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO158">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B159" t="s">
         <v>3</v>
       </c>
@@ -11582,8 +12297,14 @@
       <c r="AN159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO159">
+        <v>4</v>
+      </c>
+      <c r="AP159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B160" t="s">
         <v>3</v>
       </c>
@@ -11639,8 +12360,11 @@
       <c r="AM160">
         <v>9</v>
       </c>
-    </row>
-    <row r="161" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO160">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B161" t="s">
         <v>3</v>
       </c>
@@ -11729,8 +12453,14 @@
       <c r="AN161">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO161">
+        <v>3</v>
+      </c>
+      <c r="AP161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
         <v>3</v>
       </c>
@@ -11789,8 +12519,11 @@
       <c r="AM162">
         <v>8</v>
       </c>
-    </row>
-    <row r="163" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO162">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>1</v>
       </c>
@@ -11852,8 +12585,14 @@
       <c r="AN163">
         <v>2</v>
       </c>
-    </row>
-    <row r="164" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO163">
+        <v>4</v>
+      </c>
+      <c r="AP163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>1</v>
       </c>
@@ -11903,8 +12642,11 @@
       <c r="AM164">
         <v>9</v>
       </c>
-    </row>
-    <row r="165" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO164">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>1</v>
       </c>
@@ -11966,8 +12708,14 @@
       <c r="AN165">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO165">
+        <v>4</v>
+      </c>
+      <c r="AP165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>1</v>
       </c>
@@ -12050,8 +12798,14 @@
       <c r="AN166">
         <v>2</v>
       </c>
-    </row>
-    <row r="167" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO166">
+        <v>5</v>
+      </c>
+      <c r="AP166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
         <v>4</v>
       </c>
@@ -12101,8 +12855,14 @@
       <c r="AM167">
         <v>8</v>
       </c>
-    </row>
-    <row r="168" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO167">
+        <v>7</v>
+      </c>
+      <c r="AP167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
         <v>4</v>
       </c>
@@ -12170,8 +12930,14 @@
       <c r="AN168">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO168">
+        <v>9</v>
+      </c>
+      <c r="AP168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B169" t="s">
         <v>4</v>
       </c>
@@ -12230,8 +12996,11 @@
       <c r="AM169">
         <v>6</v>
       </c>
-    </row>
-    <row r="170" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO169">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
         <v>4</v>
       </c>
@@ -12290,8 +13059,11 @@
       <c r="AM170">
         <v>7</v>
       </c>
-    </row>
-    <row r="171" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO170">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
         <v>3</v>
       </c>
@@ -12365,8 +13137,14 @@
       <c r="AN171">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO171">
+        <v>5</v>
+      </c>
+      <c r="AP171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
         <v>3</v>
       </c>
@@ -12422,8 +13200,11 @@
       <c r="AM172">
         <v>8</v>
       </c>
-    </row>
-    <row r="173" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO172">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
         <v>3</v>
       </c>
@@ -12479,8 +13260,11 @@
       <c r="AM173">
         <v>6</v>
       </c>
-    </row>
-    <row r="174" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO173">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B174" t="s">
         <v>3</v>
       </c>
@@ -12539,8 +13323,11 @@
       <c r="AM174">
         <v>9</v>
       </c>
-    </row>
-    <row r="175" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO174">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
         <v>1</v>
       </c>
@@ -12602,8 +13389,14 @@
       <c r="AN175">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO175">
+        <v>8</v>
+      </c>
+      <c r="AP175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
         <v>1</v>
       </c>
@@ -12653,8 +13446,11 @@
       <c r="AM176">
         <v>8</v>
       </c>
-    </row>
-    <row r="177" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO176">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
         <v>1</v>
       </c>
@@ -12710,8 +13506,11 @@
       <c r="AM177">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
         <v>1</v>
       </c>
@@ -12773,8 +13572,11 @@
       <c r="AM178">
         <v>8</v>
       </c>
-    </row>
-    <row r="179" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AO178">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B179" t="s">
         <v>4</v>
       </c>
@@ -12839,8 +13641,14 @@
       <c r="AN179">
         <v>2</v>
       </c>
-    </row>
-    <row r="180" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO179">
+        <v>6</v>
+      </c>
+      <c r="AP179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B180" t="s">
         <v>4</v>
       </c>
@@ -12899,8 +13707,14 @@
       <c r="AN180">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO180">
+        <v>7</v>
+      </c>
+      <c r="AP180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
         <v>4</v>
       </c>
@@ -12956,8 +13770,11 @@
       <c r="AM181">
         <v>7</v>
       </c>
-    </row>
-    <row r="182" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO181">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
         <v>4</v>
       </c>
@@ -13016,8 +13833,11 @@
       <c r="AM182">
         <v>6</v>
       </c>
-    </row>
-    <row r="183" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO182">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
         <v>3</v>
       </c>
@@ -13096,8 +13916,14 @@
       <c r="AN183">
         <v>2</v>
       </c>
-    </row>
-    <row r="184" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO183">
+        <v>5</v>
+      </c>
+      <c r="AP183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
         <v>1</v>
       </c>
@@ -13152,8 +13978,11 @@
       <c r="AM184">
         <v>6</v>
       </c>
-    </row>
-    <row r="185" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO184">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
         <v>3</v>
       </c>
@@ -13208,8 +14037,11 @@
       <c r="AM185">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO185">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
         <v>1</v>
       </c>
@@ -13267,8 +14099,14 @@
       <c r="AN186">
         <v>1</v>
       </c>
-    </row>
-    <row r="187" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO186">
+        <v>6</v>
+      </c>
+      <c r="AP186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
         <v>4</v>
       </c>
@@ -13320,8 +14158,11 @@
       <c r="AM187">
         <v>7</v>
       </c>
-    </row>
-    <row r="188" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO187">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="188" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
         <v>4</v>
       </c>
@@ -13382,8 +14223,14 @@
       <c r="AN188">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO188">
+        <v>8</v>
+      </c>
+      <c r="AP188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
         <v>3</v>
       </c>
@@ -13468,8 +14315,14 @@
       <c r="AN189">
         <v>2</v>
       </c>
-    </row>
-    <row r="190" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO189">
+        <v>2</v>
+      </c>
+      <c r="AP189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
         <v>1</v>
       </c>
@@ -13545,8 +14398,14 @@
       <c r="AN190">
         <v>2</v>
       </c>
-    </row>
-    <row r="191" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO190">
+        <v>3</v>
+      </c>
+      <c r="AP190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
         <v>3</v>
       </c>
@@ -13622,8 +14481,14 @@
       <c r="AN191">
         <v>2</v>
       </c>
-    </row>
-    <row r="192" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO191">
+        <v>3</v>
+      </c>
+      <c r="AP191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
         <v>1</v>
       </c>
@@ -13684,8 +14549,14 @@
       <c r="AN192">
         <v>2</v>
       </c>
-    </row>
-    <row r="193" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO192">
+        <v>1</v>
+      </c>
+      <c r="AP192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B193" t="s">
         <v>4</v>
       </c>
@@ -13767,8 +14638,14 @@
       <c r="AN193">
         <v>2</v>
       </c>
-    </row>
-    <row r="194" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO193">
+        <v>5</v>
+      </c>
+      <c r="AP193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B194" t="s">
         <v>4</v>
       </c>
@@ -13826,8 +14703,14 @@
       <c r="AM194">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO194">
+        <v>4</v>
+      </c>
+      <c r="AP194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B195" t="s">
         <v>3</v>
       </c>
@@ -13909,8 +14792,14 @@
       <c r="AN195">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO195">
+        <v>2</v>
+      </c>
+      <c r="AP195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B196" t="s">
         <v>1</v>
       </c>
@@ -13998,8 +14887,14 @@
       <c r="AN196">
         <v>3</v>
       </c>
-    </row>
-    <row r="197" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO196">
+        <v>5</v>
+      </c>
+      <c r="AP196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B197" t="s">
         <v>3</v>
       </c>
@@ -14063,8 +14958,11 @@
       <c r="AM197">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B198" t="s">
         <v>1</v>
       </c>
@@ -14119,8 +15017,11 @@
       <c r="AM198">
         <v>5</v>
       </c>
-    </row>
-    <row r="199" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO198">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B199" t="s">
         <v>4</v>
       </c>
@@ -14187,8 +15088,14 @@
       <c r="AN199">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO199">
+        <v>5</v>
+      </c>
+      <c r="AP199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B200" t="s">
         <v>4</v>
       </c>
@@ -14246,8 +15153,11 @@
       <c r="AM200">
         <v>7</v>
       </c>
-    </row>
-    <row r="201" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO200">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B201" t="s">
         <v>3</v>
       </c>
@@ -14320,8 +15230,14 @@
       <c r="AN201">
         <v>2</v>
       </c>
-    </row>
-    <row r="202" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO201">
+        <v>3</v>
+      </c>
+      <c r="AP201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B202" t="s">
         <v>1</v>
       </c>
@@ -14403,8 +15319,14 @@
       <c r="AN202">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO202">
+        <v>0</v>
+      </c>
+      <c r="AP202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B203" t="s">
         <v>3</v>
       </c>
@@ -14471,8 +15393,14 @@
       <c r="AN203">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO203">
+        <v>3</v>
+      </c>
+      <c r="AP203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B204" t="s">
         <v>1</v>
       </c>
@@ -14527,8 +15455,11 @@
       <c r="AM204">
         <v>5</v>
       </c>
-    </row>
-    <row r="205" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO204">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B205" t="s">
         <v>4</v>
       </c>
@@ -14613,8 +15544,14 @@
       <c r="AN205">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO205">
+        <v>9</v>
+      </c>
+      <c r="AP205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
         <v>4</v>
       </c>
@@ -14669,8 +15606,11 @@
       <c r="AM206">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO206">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
         <v>3</v>
       </c>
@@ -14725,8 +15665,11 @@
       <c r="AM207">
         <v>4</v>
       </c>
-    </row>
-    <row r="208" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B208" t="s">
         <v>1</v>
       </c>
@@ -14802,8 +15745,14 @@
       <c r="AN208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO208">
+        <v>2</v>
+      </c>
+      <c r="AP208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B209" t="s">
         <v>3</v>
       </c>
@@ -14861,8 +15810,14 @@
       <c r="AM209">
         <v>5</v>
       </c>
-    </row>
-    <row r="210" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO209">
+        <v>4</v>
+      </c>
+      <c r="AP209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B210" t="s">
         <v>1</v>
       </c>
@@ -14944,8 +15899,14 @@
       <c r="AN210">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO210">
+        <v>4</v>
+      </c>
+      <c r="AP210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B211" t="s">
         <v>4</v>
       </c>
@@ -15003,8 +15964,14 @@
       <c r="AN211">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="2:40" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AO211">
+        <v>3</v>
+      </c>
+      <c r="AP211">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B212" t="s">
         <v>4</v>
       </c>
@@ -15059,8 +16026,11 @@
       <c r="AM212">
         <v>5</v>
       </c>
-    </row>
-    <row r="213" spans="2:40" hidden="1" x14ac:dyDescent="0.35"/>
+      <c r="AO212">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="2:42" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cleaned up datasets, and modified code to take a dataset containing both dead and alive
</commit_message>
<xml_diff>
--- a/data/germination_data.xlsx
+++ b/data/germination_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\morasoilinoculation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanmeier/git/morasoilinoculation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4C972F-59D2-4E48-B228-A858BA21171B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DFA9B0-EBE9-CA41-82FE-659C76E1605A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
+    <workbookView xWindow="4420" yWindow="680" windowWidth="19420" windowHeight="10300" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="70">
   <si>
     <t>seed_species</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSHE </t>
   </si>
   <si>
     <t>inoculated_%</t>
@@ -277,20 +274,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -354,21 +351,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AP213" totalsRowShown="0">
-  <autoFilter ref="B2:AP213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AP212" totalsRowShown="0">
+  <autoFilter ref="B2:AP212" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
     <filterColumn colId="0">
       <filters>
-        <filter val="THPL"/>
+        <filter val="TSHE"/>
       </filters>
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="PSME"/>
+        <filter val="TSHE"/>
       </filters>
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="0"/>
+        <filter val="25"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -736,20 +733,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68F8197-A530-A948-B005-AEDF71CF4B66}">
-  <dimension ref="B2:AP213"/>
+  <dimension ref="B2:AP212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="73" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="AO146" sqref="AO146"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="D220" sqref="D220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.15234375" customWidth="1"/>
-    <col min="4" max="4" width="17.84375" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -757,992 +754,992 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
       <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
       <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
       <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
       <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" t="s">
         <v>29</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>30</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>31</v>
       </c>
-      <c r="T2" t="s">
-        <v>32</v>
-      </c>
       <c r="U2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" t="s">
         <v>34</v>
       </c>
-      <c r="V2" t="s">
-        <v>35</v>
-      </c>
       <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
         <v>37</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+      <c r="U3">
+        <v>5</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>3</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>3</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>3</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>3</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>3</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>3</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
+        <v>3</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="S4">
+        <v>6</v>
+      </c>
+      <c r="U4">
+        <v>7</v>
+      </c>
+      <c r="W4">
+        <v>8</v>
+      </c>
+      <c r="Y4">
+        <v>8</v>
+      </c>
+      <c r="AA4">
+        <v>8</v>
+      </c>
+      <c r="AC4">
+        <v>9</v>
+      </c>
+      <c r="AE4">
+        <v>9</v>
+      </c>
+      <c r="AG4">
+        <v>9</v>
+      </c>
+      <c r="AI4">
+        <v>9</v>
+      </c>
+      <c r="AK4">
+        <v>9</v>
+      </c>
+      <c r="AM4">
+        <v>9</v>
+      </c>
+      <c r="AO4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="Q5">
+        <v>7</v>
+      </c>
+      <c r="S5">
+        <v>7</v>
+      </c>
+      <c r="U5">
+        <v>6</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>6</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>6</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>6</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>6</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>6</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>6</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>6</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>6</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
+        <v>6</v>
+      </c>
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
+        <v>6</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>7</v>
+      </c>
+      <c r="Q6">
+        <v>7</v>
+      </c>
+      <c r="S6">
+        <v>7</v>
+      </c>
+      <c r="U6">
+        <v>7</v>
+      </c>
+      <c r="W6">
+        <v>8</v>
+      </c>
+      <c r="Y6">
+        <v>8</v>
+      </c>
+      <c r="AA6">
+        <v>8</v>
+      </c>
+      <c r="AC6">
+        <v>8</v>
+      </c>
+      <c r="AE6">
+        <v>8</v>
+      </c>
+      <c r="AG6">
+        <v>8</v>
+      </c>
+      <c r="AI6">
+        <v>8</v>
+      </c>
+      <c r="AK6">
+        <v>8</v>
+      </c>
+      <c r="AM6">
+        <v>8</v>
+      </c>
+      <c r="AO6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AC7">
+        <v>6</v>
+      </c>
+      <c r="AE7">
+        <v>6</v>
+      </c>
+      <c r="AG7">
+        <v>6</v>
+      </c>
+      <c r="AI7">
+        <v>6</v>
+      </c>
+      <c r="AK7">
+        <v>6</v>
+      </c>
+      <c r="AM7">
+        <v>6</v>
+      </c>
+      <c r="AO7">
+        <v>5</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>5</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>6</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>6</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>6</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>6</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>6</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <v>6</v>
+      </c>
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>6</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>6</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+      <c r="W9">
+        <v>6</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>6</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>6</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>6</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>6</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>6</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>6</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>6</v>
+      </c>
+      <c r="AN9">
+        <v>1</v>
+      </c>
+      <c r="AO9">
+        <v>6</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>6</v>
+      </c>
+      <c r="U10">
+        <v>8</v>
+      </c>
+      <c r="W10">
+        <v>8</v>
+      </c>
+      <c r="Y10">
+        <v>8</v>
+      </c>
+      <c r="AA10">
+        <v>8</v>
+      </c>
+      <c r="AC10">
+        <v>8</v>
+      </c>
+      <c r="AE10">
+        <v>8</v>
+      </c>
+      <c r="AG10">
+        <v>8</v>
+      </c>
+      <c r="AI10">
+        <v>8</v>
+      </c>
+      <c r="AK10">
+        <v>8</v>
+      </c>
+      <c r="AM10">
+        <v>8</v>
+      </c>
+      <c r="AO10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>3</v>
+      </c>
+      <c r="Y11">
+        <v>7</v>
+      </c>
+      <c r="AA11">
+        <v>6</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11">
+        <v>7</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11">
+        <v>7</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>7</v>
+      </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11">
+        <v>7</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AK11">
+        <v>6</v>
+      </c>
+      <c r="AL11">
+        <v>2</v>
+      </c>
+      <c r="AM11">
+        <v>6</v>
+      </c>
+      <c r="AN11">
+        <v>2</v>
+      </c>
+      <c r="AO11">
+        <v>6</v>
+      </c>
+      <c r="AP11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>2</v>
+      </c>
+      <c r="X12">
+        <v>2</v>
+      </c>
+      <c r="Y12">
+        <v>3</v>
+      </c>
+      <c r="Z12">
+        <v>2</v>
+      </c>
+      <c r="AA12">
+        <v>3</v>
+      </c>
+      <c r="AB12">
+        <v>2</v>
+      </c>
+      <c r="AC12">
+        <v>6</v>
+      </c>
+      <c r="AD12">
+        <v>1</v>
+      </c>
+      <c r="AE12">
+        <v>6</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>6</v>
+      </c>
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
+        <v>6</v>
+      </c>
+      <c r="AJ12">
+        <v>1</v>
+      </c>
+      <c r="AK12">
+        <v>5</v>
+      </c>
+      <c r="AL12">
+        <v>2</v>
+      </c>
+      <c r="AM12">
+        <v>5</v>
+      </c>
+      <c r="AN12">
+        <v>2</v>
+      </c>
+      <c r="AO12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="S13">
+        <v>6</v>
+      </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="W13">
+        <v>5</v>
+      </c>
+      <c r="Y13">
+        <v>5</v>
+      </c>
+      <c r="AA13">
+        <v>5</v>
+      </c>
+      <c r="AC13">
+        <v>5</v>
+      </c>
+      <c r="AE13">
+        <v>5</v>
+      </c>
+      <c r="AG13">
+        <v>5</v>
+      </c>
+      <c r="AI13">
+        <v>5</v>
+      </c>
+      <c r="AK13">
+        <v>6</v>
+      </c>
+      <c r="AM13">
+        <v>6</v>
+      </c>
+      <c r="AO13">
+        <v>5</v>
+      </c>
+      <c r="AP13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="O3">
-        <v>4</v>
-      </c>
-      <c r="Q3">
-        <v>5</v>
-      </c>
-      <c r="S3">
-        <v>6</v>
-      </c>
-      <c r="U3">
-        <v>5</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>4</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>3</v>
-      </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AC3">
-        <v>3</v>
-      </c>
-      <c r="AD3">
-        <v>1</v>
-      </c>
-      <c r="AE3">
-        <v>3</v>
-      </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
-        <v>3</v>
-      </c>
-      <c r="AH3">
-        <v>1</v>
-      </c>
-      <c r="AI3">
-        <v>3</v>
-      </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AK3">
-        <v>3</v>
-      </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AM3">
-        <v>3</v>
-      </c>
-      <c r="AN3">
-        <v>1</v>
-      </c>
-      <c r="AO3">
-        <v>3</v>
-      </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>4</v>
-      </c>
-      <c r="S4">
-        <v>6</v>
-      </c>
-      <c r="U4">
-        <v>7</v>
-      </c>
-      <c r="W4">
-        <v>8</v>
-      </c>
-      <c r="Y4">
-        <v>8</v>
-      </c>
-      <c r="AA4">
-        <v>8</v>
-      </c>
-      <c r="AC4">
-        <v>9</v>
-      </c>
-      <c r="AE4">
-        <v>9</v>
-      </c>
-      <c r="AG4">
-        <v>9</v>
-      </c>
-      <c r="AI4">
-        <v>9</v>
-      </c>
-      <c r="AK4">
-        <v>9</v>
-      </c>
-      <c r="AM4">
-        <v>9</v>
-      </c>
-      <c r="AO4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>4</v>
-      </c>
-      <c r="O5">
-        <v>6</v>
-      </c>
-      <c r="Q5">
-        <v>7</v>
-      </c>
-      <c r="S5">
-        <v>7</v>
-      </c>
-      <c r="U5">
-        <v>6</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>6</v>
-      </c>
-      <c r="X5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <v>6</v>
-      </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
-      <c r="AA5">
-        <v>6</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5">
-        <v>6</v>
-      </c>
-      <c r="AD5">
-        <v>1</v>
-      </c>
-      <c r="AE5">
-        <v>6</v>
-      </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
-      <c r="AG5">
-        <v>6</v>
-      </c>
-      <c r="AH5">
-        <v>1</v>
-      </c>
-      <c r="AI5">
-        <v>6</v>
-      </c>
-      <c r="AJ5">
-        <v>1</v>
-      </c>
-      <c r="AK5">
-        <v>6</v>
-      </c>
-      <c r="AL5">
-        <v>1</v>
-      </c>
-      <c r="AM5">
-        <v>6</v>
-      </c>
-      <c r="AN5">
-        <v>1</v>
-      </c>
-      <c r="AO5">
-        <v>6</v>
-      </c>
-      <c r="AP5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>6</v>
-      </c>
-      <c r="O6">
-        <v>7</v>
-      </c>
-      <c r="Q6">
-        <v>7</v>
-      </c>
-      <c r="S6">
-        <v>7</v>
-      </c>
-      <c r="U6">
-        <v>7</v>
-      </c>
-      <c r="W6">
-        <v>8</v>
-      </c>
-      <c r="Y6">
-        <v>8</v>
-      </c>
-      <c r="AA6">
-        <v>8</v>
-      </c>
-      <c r="AC6">
-        <v>8</v>
-      </c>
-      <c r="AE6">
-        <v>8</v>
-      </c>
-      <c r="AG6">
-        <v>8</v>
-      </c>
-      <c r="AI6">
-        <v>8</v>
-      </c>
-      <c r="AK6">
-        <v>8</v>
-      </c>
-      <c r="AM6">
-        <v>8</v>
-      </c>
-      <c r="AO6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>3</v>
-      </c>
-      <c r="W7">
-        <v>3</v>
-      </c>
-      <c r="Y7">
-        <v>3</v>
-      </c>
-      <c r="AA7">
-        <v>5</v>
-      </c>
-      <c r="AC7">
-        <v>6</v>
-      </c>
-      <c r="AE7">
-        <v>6</v>
-      </c>
-      <c r="AG7">
-        <v>6</v>
-      </c>
-      <c r="AI7">
-        <v>6</v>
-      </c>
-      <c r="AK7">
-        <v>6</v>
-      </c>
-      <c r="AM7">
-        <v>6</v>
-      </c>
-      <c r="AO7">
-        <v>5</v>
-      </c>
-      <c r="AP7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>2</v>
-      </c>
-      <c r="U8">
-        <v>4</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
-        <v>5</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8">
-        <v>5</v>
-      </c>
-      <c r="Z8">
-        <v>1</v>
-      </c>
-      <c r="AA8">
-        <v>5</v>
-      </c>
-      <c r="AB8">
-        <v>1</v>
-      </c>
-      <c r="AC8">
-        <v>6</v>
-      </c>
-      <c r="AD8">
-        <v>1</v>
-      </c>
-      <c r="AE8">
-        <v>6</v>
-      </c>
-      <c r="AF8">
-        <v>1</v>
-      </c>
-      <c r="AG8">
-        <v>6</v>
-      </c>
-      <c r="AH8">
-        <v>1</v>
-      </c>
-      <c r="AI8">
-        <v>6</v>
-      </c>
-      <c r="AJ8">
-        <v>1</v>
-      </c>
-      <c r="AK8">
-        <v>6</v>
-      </c>
-      <c r="AL8">
-        <v>1</v>
-      </c>
-      <c r="AM8">
-        <v>6</v>
-      </c>
-      <c r="AN8">
-        <v>1</v>
-      </c>
-      <c r="AO8">
-        <v>6</v>
-      </c>
-      <c r="AP8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="O9">
-        <v>5</v>
-      </c>
-      <c r="Q9">
-        <v>5</v>
-      </c>
-      <c r="S9">
-        <v>6</v>
-      </c>
-      <c r="U9">
-        <v>6</v>
-      </c>
-      <c r="W9">
-        <v>6</v>
-      </c>
-      <c r="X9">
-        <v>1</v>
-      </c>
-      <c r="Y9">
-        <v>6</v>
-      </c>
-      <c r="Z9">
-        <v>1</v>
-      </c>
-      <c r="AA9">
-        <v>6</v>
-      </c>
-      <c r="AB9">
-        <v>1</v>
-      </c>
-      <c r="AC9">
-        <v>6</v>
-      </c>
-      <c r="AD9">
-        <v>1</v>
-      </c>
-      <c r="AE9">
-        <v>6</v>
-      </c>
-      <c r="AF9">
-        <v>1</v>
-      </c>
-      <c r="AG9">
-        <v>6</v>
-      </c>
-      <c r="AH9">
-        <v>1</v>
-      </c>
-      <c r="AI9">
-        <v>6</v>
-      </c>
-      <c r="AJ9">
-        <v>1</v>
-      </c>
-      <c r="AK9">
-        <v>6</v>
-      </c>
-      <c r="AL9">
-        <v>1</v>
-      </c>
-      <c r="AM9">
-        <v>6</v>
-      </c>
-      <c r="AN9">
-        <v>1</v>
-      </c>
-      <c r="AO9">
-        <v>6</v>
-      </c>
-      <c r="AP9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="Q10">
-        <v>4</v>
-      </c>
-      <c r="S10">
-        <v>6</v>
-      </c>
-      <c r="U10">
-        <v>8</v>
-      </c>
-      <c r="W10">
-        <v>8</v>
-      </c>
-      <c r="Y10">
-        <v>8</v>
-      </c>
-      <c r="AA10">
-        <v>8</v>
-      </c>
-      <c r="AC10">
-        <v>8</v>
-      </c>
-      <c r="AE10">
-        <v>8</v>
-      </c>
-      <c r="AG10">
-        <v>8</v>
-      </c>
-      <c r="AI10">
-        <v>8</v>
-      </c>
-      <c r="AK10">
-        <v>8</v>
-      </c>
-      <c r="AM10">
-        <v>8</v>
-      </c>
-      <c r="AO10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>3</v>
-      </c>
-      <c r="Y11">
-        <v>7</v>
-      </c>
-      <c r="AA11">
-        <v>6</v>
-      </c>
-      <c r="AB11">
-        <v>1</v>
-      </c>
-      <c r="AC11">
-        <v>7</v>
-      </c>
-      <c r="AD11">
-        <v>1</v>
-      </c>
-      <c r="AE11">
-        <v>7</v>
-      </c>
-      <c r="AF11">
-        <v>1</v>
-      </c>
-      <c r="AG11">
-        <v>7</v>
-      </c>
-      <c r="AH11">
-        <v>1</v>
-      </c>
-      <c r="AI11">
-        <v>7</v>
-      </c>
-      <c r="AJ11">
-        <v>1</v>
-      </c>
-      <c r="AK11">
-        <v>6</v>
-      </c>
-      <c r="AL11">
-        <v>2</v>
-      </c>
-      <c r="AM11">
-        <v>6</v>
-      </c>
-      <c r="AN11">
-        <v>2</v>
-      </c>
-      <c r="AO11">
-        <v>6</v>
-      </c>
-      <c r="AP11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>2</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12">
-        <v>3</v>
-      </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
-      <c r="W12">
-        <v>2</v>
-      </c>
-      <c r="X12">
-        <v>2</v>
-      </c>
-      <c r="Y12">
-        <v>3</v>
-      </c>
-      <c r="Z12">
-        <v>2</v>
-      </c>
-      <c r="AA12">
-        <v>3</v>
-      </c>
-      <c r="AB12">
-        <v>2</v>
-      </c>
-      <c r="AC12">
-        <v>6</v>
-      </c>
-      <c r="AD12">
-        <v>1</v>
-      </c>
-      <c r="AE12">
-        <v>6</v>
-      </c>
-      <c r="AF12">
-        <v>1</v>
-      </c>
-      <c r="AG12">
-        <v>6</v>
-      </c>
-      <c r="AH12">
-        <v>1</v>
-      </c>
-      <c r="AI12">
-        <v>6</v>
-      </c>
-      <c r="AJ12">
-        <v>1</v>
-      </c>
-      <c r="AK12">
-        <v>5</v>
-      </c>
-      <c r="AL12">
-        <v>2</v>
-      </c>
-      <c r="AM12">
-        <v>5</v>
-      </c>
-      <c r="AN12">
-        <v>2</v>
-      </c>
-      <c r="AO12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>2</v>
-      </c>
-      <c r="O13">
-        <v>5</v>
-      </c>
-      <c r="Q13">
-        <v>5</v>
-      </c>
-      <c r="S13">
-        <v>6</v>
-      </c>
-      <c r="U13">
-        <v>5</v>
-      </c>
-      <c r="W13">
-        <v>5</v>
-      </c>
-      <c r="Y13">
-        <v>5</v>
-      </c>
-      <c r="AA13">
-        <v>5</v>
-      </c>
-      <c r="AC13">
-        <v>5</v>
-      </c>
-      <c r="AE13">
-        <v>5</v>
-      </c>
-      <c r="AG13">
-        <v>5</v>
-      </c>
-      <c r="AI13">
-        <v>5</v>
-      </c>
-      <c r="AK13">
-        <v>6</v>
-      </c>
-      <c r="AM13">
-        <v>6</v>
-      </c>
-      <c r="AO13">
-        <v>5</v>
-      </c>
-      <c r="AP13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="K14">
         <v>2</v>
       </c>
@@ -1810,7 +1807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1825,7 +1822,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M15">
         <v>2</v>
@@ -1882,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1957,7 +1954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -2038,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -2095,7 +2092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -2110,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q19">
         <v>4</v>
@@ -2179,7 +2176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -2236,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -2298,7 +2295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -2313,7 +2310,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -2361,7 +2358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -2418,7 +2415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -2433,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -2481,7 +2478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -2541,7 +2538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -2556,7 +2553,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I26">
         <v>3</v>
@@ -2649,7 +2646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -2664,7 +2661,7 @@
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M27">
         <v>4</v>
@@ -2712,7 +2709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -2805,7 +2802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -2865,7 +2862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -2880,7 +2877,7 @@
         <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -2931,7 +2928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -3021,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -3075,7 +3072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -3138,7 +3135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -3153,7 +3150,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -3228,7 +3225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -3243,7 +3240,7 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O35">
         <v>2</v>
@@ -3297,7 +3294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -3312,7 +3309,7 @@
         <v>3</v>
       </c>
       <c r="F36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O36">
         <v>1</v>
@@ -3372,7 +3369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -3432,7 +3429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>4</v>
       </c>
@@ -3447,7 +3444,7 @@
         <v>3</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K38">
         <v>3</v>
@@ -3540,7 +3537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3630,7 +3627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -3645,7 +3642,7 @@
         <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M40">
         <v>1</v>
@@ -3732,7 +3729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -3801,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -3816,7 +3813,7 @@
         <v>4</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -3870,7 +3867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>1</v>
       </c>
@@ -3957,7 +3954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>1</v>
       </c>
@@ -4011,7 +4008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -4026,7 +4023,7 @@
         <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I45">
         <v>2</v>
@@ -4125,7 +4122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>1</v>
       </c>
@@ -4140,7 +4137,7 @@
         <v>4</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K46">
         <v>2</v>
@@ -4191,7 +4188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -4206,7 +4203,7 @@
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O47">
         <v>1</v>
@@ -4251,7 +4248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>4</v>
       </c>
@@ -4266,7 +4263,7 @@
         <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M48">
         <v>1</v>
@@ -4350,7 +4347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -4410,7 +4407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -4425,7 +4422,7 @@
         <v>4</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I50">
         <v>1</v>
@@ -4524,7 +4521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -4539,7 +4536,7 @@
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -4611,7 +4608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -4671,7 +4668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -4749,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -4812,7 +4809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>1</v>
       </c>
@@ -4884,7 +4881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>1</v>
       </c>
@@ -4938,7 +4935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -4998,7 +4995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>1</v>
       </c>
@@ -5013,7 +5010,7 @@
         <v>5</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K58">
         <v>1</v>
@@ -5064,7 +5061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>4</v>
       </c>
@@ -5121,7 +5118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>4</v>
       </c>
@@ -5136,7 +5133,7 @@
         <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O60">
         <v>1</v>
@@ -5193,7 +5190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>4</v>
       </c>
@@ -5253,7 +5250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>4</v>
       </c>
@@ -5268,7 +5265,7 @@
         <v>5</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K62">
         <v>2</v>
@@ -5355,7 +5352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>3</v>
       </c>
@@ -5370,7 +5367,7 @@
         <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M63">
         <v>1</v>
@@ -5436,7 +5433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>3</v>
       </c>
@@ -5499,7 +5496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -5559,7 +5556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>3</v>
       </c>
@@ -5619,7 +5616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -5709,7 +5706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -5763,7 +5760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>1</v>
       </c>
@@ -5823,7 +5820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>1</v>
       </c>
@@ -5838,7 +5835,7 @@
         <v>6</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I70">
         <v>1</v>
@@ -5892,7 +5889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>4</v>
       </c>
@@ -5907,7 +5904,7 @@
         <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O71">
         <v>4</v>
@@ -5961,7 +5958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>4</v>
       </c>
@@ -5976,7 +5973,7 @@
         <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O72">
         <v>2</v>
@@ -6042,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>4</v>
       </c>
@@ -6102,7 +6099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>4</v>
       </c>
@@ -6117,7 +6114,7 @@
         <v>6</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I74">
         <v>3</v>
@@ -6171,7 +6168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>3</v>
       </c>
@@ -6186,7 +6183,7 @@
         <v>7</v>
       </c>
       <c r="F75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M75">
         <v>1</v>
@@ -6237,7 +6234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>3</v>
       </c>
@@ -6252,7 +6249,7 @@
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M76">
         <v>1</v>
@@ -6336,7 +6333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>3</v>
       </c>
@@ -6399,7 +6396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>3</v>
       </c>
@@ -6414,7 +6411,7 @@
         <v>7</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M78">
         <v>2</v>
@@ -6462,7 +6459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>1</v>
       </c>
@@ -6555,7 +6552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>1</v>
       </c>
@@ -6618,7 +6615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>1</v>
       </c>
@@ -6633,7 +6630,7 @@
         <v>7</v>
       </c>
       <c r="F81" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K81">
         <v>4</v>
@@ -6693,7 +6690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>1</v>
       </c>
@@ -6708,7 +6705,7 @@
         <v>7</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K82">
         <v>2</v>
@@ -6789,7 +6786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>4</v>
       </c>
@@ -6804,7 +6801,7 @@
         <v>7</v>
       </c>
       <c r="F83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O83">
         <v>2</v>
@@ -6882,7 +6879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>4</v>
       </c>
@@ -6897,7 +6894,7 @@
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O84">
         <v>2</v>
@@ -6975,7 +6972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>4</v>
       </c>
@@ -6990,7 +6987,7 @@
         <v>7</v>
       </c>
       <c r="F85" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M85">
         <v>3</v>
@@ -7065,7 +7062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>4</v>
       </c>
@@ -7080,7 +7077,7 @@
         <v>7</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I86">
         <v>2</v>
@@ -7137,7 +7134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>3</v>
       </c>
@@ -7152,7 +7149,7 @@
         <v>8</v>
       </c>
       <c r="F87" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M87">
         <v>2</v>
@@ -7233,7 +7230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>3</v>
       </c>
@@ -7248,7 +7245,7 @@
         <v>8</v>
       </c>
       <c r="F88" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M88">
         <v>0</v>
@@ -7314,7 +7311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>3</v>
       </c>
@@ -7377,7 +7374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>3</v>
       </c>
@@ -7440,7 +7437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>1</v>
       </c>
@@ -7530,7 +7527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>1</v>
       </c>
@@ -7599,7 +7596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>1</v>
       </c>
@@ -7662,7 +7659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>1</v>
       </c>
@@ -7677,7 +7674,7 @@
         <v>8</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K94">
         <v>2</v>
@@ -7728,7 +7725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>4</v>
       </c>
@@ -7743,7 +7740,7 @@
         <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O95">
         <v>2</v>
@@ -7788,7 +7785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>4</v>
       </c>
@@ -7803,7 +7800,7 @@
         <v>8</v>
       </c>
       <c r="F96" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O96">
         <v>1</v>
@@ -7863,7 +7860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>4</v>
       </c>
@@ -7878,7 +7875,7 @@
         <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M97">
         <v>4</v>
@@ -7926,7 +7923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>4</v>
       </c>
@@ -7941,7 +7938,7 @@
         <v>8</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K98">
         <v>1</v>
@@ -8001,7 +7998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>3</v>
       </c>
@@ -8058,7 +8055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>3</v>
       </c>
@@ -8118,7 +8115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>3</v>
       </c>
@@ -8133,7 +8130,7 @@
         <v>9</v>
       </c>
       <c r="F101" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M101">
         <v>1</v>
@@ -8181,7 +8178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>3</v>
       </c>
@@ -8244,7 +8241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>1</v>
       </c>
@@ -8259,7 +8256,7 @@
         <v>9</v>
       </c>
       <c r="F103" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q103">
         <v>1</v>
@@ -8328,7 +8325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>1</v>
       </c>
@@ -8385,7 +8382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>1</v>
       </c>
@@ -8454,7 +8451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>1</v>
       </c>
@@ -8469,7 +8466,7 @@
         <v>9</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K106">
         <v>0</v>
@@ -8544,7 +8541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>4</v>
       </c>
@@ -8625,7 +8622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>4</v>
       </c>
@@ -8640,7 +8637,7 @@
         <v>9</v>
       </c>
       <c r="F108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q108">
         <v>3</v>
@@ -8682,7 +8679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>4</v>
       </c>
@@ -8751,7 +8748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>4</v>
       </c>
@@ -8766,7 +8763,7 @@
         <v>9</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K110">
         <v>4</v>
@@ -8832,7 +8829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>3</v>
       </c>
@@ -8847,7 +8844,7 @@
         <v>10</v>
       </c>
       <c r="F111" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G111">
         <v>1</v>
@@ -8895,7 +8892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>3</v>
       </c>
@@ -8970,7 +8967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>3</v>
       </c>
@@ -9060,7 +9057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>3</v>
       </c>
@@ -9123,7 +9120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>1</v>
       </c>
@@ -9138,7 +9135,7 @@
         <v>10</v>
       </c>
       <c r="F115" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O115">
         <v>2</v>
@@ -9216,7 +9213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>1</v>
       </c>
@@ -9273,7 +9270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>1</v>
       </c>
@@ -9342,7 +9339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>1</v>
       </c>
@@ -9409,7 +9406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>4</v>
       </c>
@@ -9466,7 +9463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>4</v>
       </c>
@@ -9481,7 +9478,7 @@
         <v>10</v>
       </c>
       <c r="F120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O120">
         <v>1</v>
@@ -9526,7 +9523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>4</v>
       </c>
@@ -9541,7 +9538,7 @@
         <v>10</v>
       </c>
       <c r="F121" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M121">
         <v>3</v>
@@ -9589,7 +9586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>4</v>
       </c>
@@ -9604,7 +9601,7 @@
         <v>10</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K122">
         <v>2</v>
@@ -9655,7 +9652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -9727,7 +9724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>3</v>
       </c>
@@ -9742,7 +9739,7 @@
         <v>11</v>
       </c>
       <c r="F124" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M124">
         <v>1</v>
@@ -9826,7 +9823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>3</v>
       </c>
@@ -9841,7 +9838,7 @@
         <v>11</v>
       </c>
       <c r="F125" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M125">
         <v>2</v>
@@ -9925,7 +9922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>3</v>
       </c>
@@ -10003,7 +10000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>1</v>
       </c>
@@ -10078,7 +10075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>1</v>
       </c>
@@ -10132,7 +10129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>1</v>
       </c>
@@ -10207,7 +10204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>1</v>
       </c>
@@ -10222,7 +10219,7 @@
         <v>11</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K130">
         <v>0</v>
@@ -10273,7 +10270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>4</v>
       </c>
@@ -10288,7 +10285,7 @@
         <v>11</v>
       </c>
       <c r="F131" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q131">
         <v>2</v>
@@ -10339,7 +10336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>4</v>
       </c>
@@ -10354,7 +10351,7 @@
         <v>11</v>
       </c>
       <c r="F132" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q132">
         <v>0</v>
@@ -10396,7 +10393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>4</v>
       </c>
@@ -10456,7 +10453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>4</v>
       </c>
@@ -10471,7 +10468,7 @@
         <v>11</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I134">
         <v>1</v>
@@ -10525,7 +10522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>3</v>
       </c>
@@ -10585,7 +10582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>3</v>
       </c>
@@ -10645,7 +10642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>3</v>
       </c>
@@ -10708,7 +10705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>3</v>
       </c>
@@ -10789,7 +10786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>1</v>
       </c>
@@ -10852,7 +10849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>1</v>
       </c>
@@ -10906,7 +10903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>1</v>
       </c>
@@ -10921,7 +10918,7 @@
         <v>12</v>
       </c>
       <c r="F141" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K141">
         <v>1</v>
@@ -11008,7 +11005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>1</v>
       </c>
@@ -11023,7 +11020,7 @@
         <v>12</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K142">
         <v>1</v>
@@ -11107,7 +11104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>4</v>
       </c>
@@ -11161,7 +11158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>4</v>
       </c>
@@ -11176,7 +11173,7 @@
         <v>12</v>
       </c>
       <c r="F144" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q144">
         <v>0</v>
@@ -11218,7 +11215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>4</v>
       </c>
@@ -11281,7 +11278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>4</v>
       </c>
@@ -11296,7 +11293,7 @@
         <v>12</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I146">
         <v>2</v>
@@ -11371,7 +11368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>3</v>
       </c>
@@ -11386,7 +11383,7 @@
         <v>13</v>
       </c>
       <c r="F147" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O147">
         <v>0</v>
@@ -11455,7 +11452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>3</v>
       </c>
@@ -11515,7 +11512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>3</v>
       </c>
@@ -11590,7 +11587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>3</v>
       </c>
@@ -11605,7 +11602,7 @@
         <v>13</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K150">
         <v>2</v>
@@ -11686,7 +11683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>1</v>
       </c>
@@ -11701,7 +11698,7 @@
         <v>13</v>
       </c>
       <c r="F151" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q151">
         <v>1</v>
@@ -11743,7 +11740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>1</v>
       </c>
@@ -11797,7 +11794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>1</v>
       </c>
@@ -11863,7 +11860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>1</v>
       </c>
@@ -11878,7 +11875,7 @@
         <v>13</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K154">
         <v>0</v>
@@ -11968,7 +11965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>4</v>
       </c>
@@ -12040,7 +12037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>4</v>
       </c>
@@ -12055,7 +12052,7 @@
         <v>13</v>
       </c>
       <c r="F156" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O156">
         <v>2</v>
@@ -12100,7 +12097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>4</v>
       </c>
@@ -12115,7 +12112,7 @@
         <v>13</v>
       </c>
       <c r="F157" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M157">
         <v>3</v>
@@ -12163,7 +12160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>4</v>
       </c>
@@ -12178,7 +12175,7 @@
         <v>13</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I158">
         <v>1</v>
@@ -12232,7 +12229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>3</v>
       </c>
@@ -12304,7 +12301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>3</v>
       </c>
@@ -12364,7 +12361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>3</v>
       </c>
@@ -12460,7 +12457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>3</v>
       </c>
@@ -12523,7 +12520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>1</v>
       </c>
@@ -12592,7 +12589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>1</v>
       </c>
@@ -12646,7 +12643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>1</v>
       </c>
@@ -12715,7 +12712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>1</v>
       </c>
@@ -12730,7 +12727,7 @@
         <v>14</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K166">
         <v>0</v>
@@ -12805,7 +12802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>4</v>
       </c>
@@ -12862,7 +12859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>4</v>
       </c>
@@ -12877,7 +12874,7 @@
         <v>14</v>
       </c>
       <c r="F168" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O168">
         <v>1</v>
@@ -12937,7 +12934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>4</v>
       </c>
@@ -12952,7 +12949,7 @@
         <v>14</v>
       </c>
       <c r="F169" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M169">
         <v>2</v>
@@ -13000,7 +12997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>4</v>
       </c>
@@ -13063,7 +13060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>3</v>
       </c>
@@ -13078,7 +13075,7 @@
         <v>15</v>
       </c>
       <c r="F171" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O171">
         <v>2</v>
@@ -13144,7 +13141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>3</v>
       </c>
@@ -13204,7 +13201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>3</v>
       </c>
@@ -13264,7 +13261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>3</v>
       </c>
@@ -13327,7 +13324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>1</v>
       </c>
@@ -13396,7 +13393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>1</v>
       </c>
@@ -13450,7 +13447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>1</v>
       </c>
@@ -13510,7 +13507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>1</v>
       </c>
@@ -13525,7 +13522,7 @@
         <v>15</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K178">
         <v>1</v>
@@ -13576,7 +13573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>4</v>
       </c>
@@ -13648,7 +13645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>4</v>
       </c>
@@ -13663,7 +13660,7 @@
         <v>15</v>
       </c>
       <c r="F180" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O180">
         <v>1</v>
@@ -13714,7 +13711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>4</v>
       </c>
@@ -13774,7 +13771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>4</v>
       </c>
@@ -13837,12 +13834,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>3</v>
       </c>
       <c r="C183" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D183">
         <v>25</v>
@@ -13851,7 +13848,7 @@
         <v>1</v>
       </c>
       <c r="F183" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O183">
         <v>0</v>
@@ -13923,7 +13920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>1</v>
       </c>
@@ -13982,7 +13979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>3</v>
       </c>
@@ -14041,7 +14038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>1</v>
       </c>
@@ -14106,7 +14103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>4</v>
       </c>
@@ -14162,7 +14159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>4</v>
       </c>
@@ -14230,12 +14227,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>3</v>
       </c>
       <c r="C189" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D189">
         <v>25</v>
@@ -14244,7 +14241,7 @@
         <v>2</v>
       </c>
       <c r="F189" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O189">
         <v>0</v>
@@ -14322,7 +14319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>1</v>
       </c>
@@ -14336,7 +14333,7 @@
         <v>2</v>
       </c>
       <c r="F190" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M190">
         <v>0</v>
@@ -14405,7 +14402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>3</v>
       </c>
@@ -14419,7 +14416,7 @@
         <v>2</v>
       </c>
       <c r="F191" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K191">
         <v>1</v>
@@ -14488,7 +14485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>1</v>
       </c>
@@ -14556,7 +14553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>4</v>
       </c>
@@ -14645,7 +14642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>4</v>
       </c>
@@ -14710,12 +14707,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>3</v>
       </c>
       <c r="C195" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D195">
         <v>25</v>
@@ -14724,7 +14721,7 @@
         <v>3</v>
       </c>
       <c r="F195" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O195">
         <v>0</v>
@@ -14799,7 +14796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>1</v>
       </c>
@@ -14813,7 +14810,7 @@
         <v>3</v>
       </c>
       <c r="F196" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K196">
         <v>1</v>
@@ -14894,7 +14891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>3</v>
       </c>
@@ -14962,7 +14959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>1</v>
       </c>
@@ -15021,7 +15018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>4</v>
       </c>
@@ -15095,7 +15092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>4</v>
       </c>
@@ -15157,12 +15154,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>3</v>
       </c>
       <c r="C201" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D201">
         <v>25</v>
@@ -15171,7 +15168,7 @@
         <v>4</v>
       </c>
       <c r="F201" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O201">
         <v>0</v>
@@ -15237,7 +15234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>1</v>
       </c>
@@ -15251,7 +15248,7 @@
         <v>4</v>
       </c>
       <c r="F202" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M202">
         <v>0</v>
@@ -15326,7 +15323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
         <v>3</v>
       </c>
@@ -15400,7 +15397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
         <v>1</v>
       </c>
@@ -15459,7 +15456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
         <v>4</v>
       </c>
@@ -15551,7 +15548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
         <v>4</v>
       </c>
@@ -15610,12 +15607,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
         <v>3</v>
       </c>
       <c r="C207" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D207">
         <v>25</v>
@@ -15624,7 +15621,7 @@
         <v>5</v>
       </c>
       <c r="F207" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O207">
         <v>1</v>
@@ -15669,7 +15666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
         <v>1</v>
       </c>
@@ -15752,7 +15749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
         <v>3</v>
       </c>
@@ -15766,7 +15763,7 @@
         <v>5</v>
       </c>
       <c r="F209" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M209">
         <v>1</v>
@@ -15817,7 +15814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
         <v>1</v>
       </c>
@@ -15906,7 +15903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
         <v>4</v>
       </c>
@@ -15971,7 +15968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:42" hidden="1" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
         <v>4</v>
       </c>
@@ -16030,7 +16027,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="2:42" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DOY 7 data collection
</commit_message>
<xml_diff>
--- a/data/germination_data.xlsx
+++ b/data/germination_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\morasoilinoculation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D6A162-7A3F-4101-AFD9-20E0E85A76A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486557E8-FAC3-41E1-8E6A-4894F3140D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
+    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8DD11EFF-0136-EA44-86B7-80FED636BE50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="73">
   <si>
     <t>seed_species</t>
   </si>
@@ -268,6 +268,14 @@
     <t>365_dead</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>7_alive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7_dead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -354,25 +362,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AP213" totalsRowShown="0">
-  <autoFilter ref="B2:AP213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="PSME"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TSHE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="10"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}" name="Table1" displayName="Table1" ref="B2:AR213" totalsRowShown="0">
+  <autoFilter ref="B2:AR213" xr:uid="{7BC992C1-6373-AD4D-8EE4-164E75FC3419}"/>
+  <tableColumns count="43">
     <tableColumn id="1" xr3:uid="{1199D7AD-452C-9D4F-9453-306631F01BCC}" name="soil_species"/>
     <tableColumn id="2" xr3:uid="{11F49906-5A0D-4E4F-BA5C-F91CB62A2174}" name="seed_species"/>
     <tableColumn id="3" xr3:uid="{B695F4B4-8561-9D48-9FF3-12A40CB2B7C7}" name="inoculated_%"/>
@@ -414,6 +406,8 @@
     <tableColumn id="39" xr3:uid="{26B0383B-95B6-4DD5-B7B4-685313FCC697}" name="358_dead2"/>
     <tableColumn id="40" xr3:uid="{77E0EA7E-1234-4ADB-9C12-30309866C064}" name="365_alive"/>
     <tableColumn id="41" xr3:uid="{B72A1CA6-FECC-4A5F-8AE4-79F078A65708}" name="365_dead"/>
+    <tableColumn id="42" xr3:uid="{76907406-3640-4FAB-BAFF-AC06D5B46E9A}" name="7_alive"/>
+    <tableColumn id="43" xr3:uid="{8D9570D3-D194-4003-B294-96403E3A2C6E}" name="7_dead"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -736,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68F8197-A530-A948-B005-AEDF71CF4B66}">
-  <dimension ref="B2:AP213"/>
+  <dimension ref="B2:AR212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="73" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1:AR1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AG109" zoomScale="73" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="AS10" sqref="AS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -749,7 +743,7 @@
     <col min="4" max="4" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -873,8 +867,14 @@
       <c r="AP2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -965,8 +965,14 @@
       <c r="AP3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ3">
+        <v>3</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1027,8 +1033,11 @@
       <c r="AO4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1119,8 +1128,14 @@
       <c r="AP5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ5">
+        <v>6</v>
+      </c>
+      <c r="AR5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1181,8 +1196,11 @@
       <c r="AO6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -1240,8 +1258,14 @@
       <c r="AP7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ7">
+        <v>5</v>
+      </c>
+      <c r="AR7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -1326,8 +1350,14 @@
       <c r="AP8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ8">
+        <v>6</v>
+      </c>
+      <c r="AR8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1418,8 +1448,14 @@
       <c r="AP9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ9">
+        <v>6</v>
+      </c>
+      <c r="AR9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1483,8 +1519,11 @@
       <c r="AO10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1569,8 +1608,14 @@
       <c r="AP11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ11">
+        <v>6</v>
+      </c>
+      <c r="AR11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -1664,8 +1709,14 @@
       <c r="AP12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ12">
+        <v>4</v>
+      </c>
+      <c r="AR12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1729,8 +1780,14 @@
       <c r="AP13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ13">
+        <v>5</v>
+      </c>
+      <c r="AR13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -1812,8 +1869,11 @@
       <c r="AO14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1884,8 +1944,14 @@
       <c r="AP15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ15">
+        <v>5</v>
+      </c>
+      <c r="AR15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1959,8 +2025,11 @@
       <c r="AO16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -2040,8 +2109,14 @@
       <c r="AP17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ17">
+        <v>6</v>
+      </c>
+      <c r="AR17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -2097,8 +2172,11 @@
       <c r="AO18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -2181,8 +2259,14 @@
       <c r="AP19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ19">
+        <v>3</v>
+      </c>
+      <c r="AR19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -2238,8 +2322,14 @@
       <c r="AP20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ20">
+        <v>13</v>
+      </c>
+      <c r="AR20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -2300,8 +2390,14 @@
       <c r="AP21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ21">
+        <v>5</v>
+      </c>
+      <c r="AR21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -2363,8 +2459,11 @@
       <c r="AO22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -2432,8 +2531,14 @@
       <c r="AP23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ23">
+        <v>8</v>
+      </c>
+      <c r="AR23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -2495,8 +2600,14 @@
       <c r="AP24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ24">
+        <v>8</v>
+      </c>
+      <c r="AR24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -2555,8 +2666,11 @@
       <c r="AO25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -2669,8 +2783,14 @@
       <c r="AP26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ26">
+        <v>8</v>
+      </c>
+      <c r="AR26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -2732,8 +2852,11 @@
       <c r="AO27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -2825,8 +2948,14 @@
       <c r="AP28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ28">
+        <v>7</v>
+      </c>
+      <c r="AR28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -2885,8 +3014,14 @@
       <c r="AO29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ29">
+        <v>3</v>
+      </c>
+      <c r="AR29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -2951,8 +3086,11 @@
       <c r="AO30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -3041,8 +3179,14 @@
       <c r="AP31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ31">
+        <v>4</v>
+      </c>
+      <c r="AR31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -3095,8 +3239,14 @@
       <c r="AO32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ32">
+        <v>9</v>
+      </c>
+      <c r="AR32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -3158,8 +3308,11 @@
       <c r="AO33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -3248,8 +3401,11 @@
       <c r="AO34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -3317,8 +3473,14 @@
       <c r="AP35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ35">
+        <v>6</v>
+      </c>
+      <c r="AR35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -3392,8 +3554,11 @@
       <c r="AO36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -3452,8 +3617,11 @@
       <c r="AO37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>4</v>
       </c>
@@ -3560,8 +3728,14 @@
       <c r="AP38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ38">
+        <v>5</v>
+      </c>
+      <c r="AR38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3650,8 +3824,14 @@
       <c r="AP39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ39">
+        <v>2</v>
+      </c>
+      <c r="AR39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -3752,8 +3932,14 @@
       <c r="AP40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ40">
+        <v>6</v>
+      </c>
+      <c r="AR40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -3821,8 +4007,14 @@
       <c r="AP41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ41">
+        <v>4</v>
+      </c>
+      <c r="AR41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -3890,8 +4082,11 @@
       <c r="AO42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>1</v>
       </c>
@@ -3977,8 +4172,14 @@
       <c r="AP43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ43">
+        <v>7</v>
+      </c>
+      <c r="AR43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>1</v>
       </c>
@@ -4031,8 +4232,11 @@
       <c r="AO44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -4145,8 +4349,14 @@
       <c r="AP45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ45">
+        <v>7</v>
+      </c>
+      <c r="AR45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>1</v>
       </c>
@@ -4211,8 +4421,11 @@
       <c r="AO46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -4271,8 +4484,11 @@
       <c r="AO47">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ47">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>4</v>
       </c>
@@ -4370,8 +4586,14 @@
       <c r="AP48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ48">
+        <v>7</v>
+      </c>
+      <c r="AR48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -4430,8 +4652,11 @@
       <c r="AO49">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -4544,8 +4769,14 @@
       <c r="AP50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ50">
+        <v>7</v>
+      </c>
+      <c r="AR50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -4631,8 +4862,14 @@
       <c r="AP51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ51">
+        <v>4</v>
+      </c>
+      <c r="AR51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -4691,8 +4928,11 @@
       <c r="AO52">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -4769,8 +5009,14 @@
       <c r="AP53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ53">
+        <v>2</v>
+      </c>
+      <c r="AR53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -4832,8 +5078,11 @@
       <c r="AO54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>1</v>
       </c>
@@ -4904,8 +5153,14 @@
       <c r="AP55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ55">
+        <v>4</v>
+      </c>
+      <c r="AR55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>1</v>
       </c>
@@ -4958,8 +5213,11 @@
       <c r="AO56">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -5018,8 +5276,11 @@
       <c r="AO57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>1</v>
       </c>
@@ -5084,8 +5345,11 @@
       <c r="AO58">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>4</v>
       </c>
@@ -5141,8 +5405,11 @@
       <c r="AO59">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>4</v>
       </c>
@@ -5213,8 +5480,14 @@
       <c r="AP60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ60">
+        <v>7</v>
+      </c>
+      <c r="AR60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>4</v>
       </c>
@@ -5273,8 +5546,11 @@
       <c r="AO61">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>4</v>
       </c>
@@ -5375,8 +5651,14 @@
       <c r="AP62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ62">
+        <v>3</v>
+      </c>
+      <c r="AR62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>3</v>
       </c>
@@ -5456,8 +5738,14 @@
       <c r="AP63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ63">
+        <v>6</v>
+      </c>
+      <c r="AR63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>3</v>
       </c>
@@ -5519,8 +5807,11 @@
       <c r="AO64">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -5579,8 +5870,11 @@
       <c r="AO65">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>3</v>
       </c>
@@ -5639,8 +5933,11 @@
       <c r="AO66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -5729,8 +6026,14 @@
       <c r="AP67">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ67">
+        <v>7</v>
+      </c>
+      <c r="AR67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -5783,8 +6086,11 @@
       <c r="AO68">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ68">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>1</v>
       </c>
@@ -5843,8 +6149,11 @@
       <c r="AO69">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ69">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>1</v>
       </c>
@@ -5912,8 +6221,11 @@
       <c r="AO70">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>4</v>
       </c>
@@ -5981,8 +6293,14 @@
       <c r="AP71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ71">
+        <v>8</v>
+      </c>
+      <c r="AR71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>4</v>
       </c>
@@ -6062,8 +6380,14 @@
       <c r="AP72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ72">
+        <v>6</v>
+      </c>
+      <c r="AR72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>4</v>
       </c>
@@ -6122,8 +6446,11 @@
       <c r="AO73">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>4</v>
       </c>
@@ -6191,8 +6518,11 @@
       <c r="AO74">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>3</v>
       </c>
@@ -6257,8 +6587,14 @@
       <c r="AP75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ75">
+        <v>6</v>
+      </c>
+      <c r="AR75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>3</v>
       </c>
@@ -6356,8 +6692,14 @@
       <c r="AP76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ76">
+        <v>7</v>
+      </c>
+      <c r="AR76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>3</v>
       </c>
@@ -6419,8 +6761,11 @@
       <c r="AO77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ77">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>3</v>
       </c>
@@ -6482,8 +6827,11 @@
       <c r="AO78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>1</v>
       </c>
@@ -6575,8 +6923,14 @@
       <c r="AP79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ79">
+        <v>7</v>
+      </c>
+      <c r="AR79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>1</v>
       </c>
@@ -6638,8 +6992,14 @@
       <c r="AP80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ80">
+        <v>9</v>
+      </c>
+      <c r="AR80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>1</v>
       </c>
@@ -6713,8 +7073,14 @@
       <c r="AP81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ81">
+        <v>4</v>
+      </c>
+      <c r="AR81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>1</v>
       </c>
@@ -6809,8 +7175,14 @@
       <c r="AP82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ82">
+        <v>7</v>
+      </c>
+      <c r="AR82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>4</v>
       </c>
@@ -6902,8 +7274,14 @@
       <c r="AP83">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ83">
+        <v>5</v>
+      </c>
+      <c r="AR83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>4</v>
       </c>
@@ -6995,8 +7373,14 @@
       <c r="AP84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ84">
+        <v>7</v>
+      </c>
+      <c r="AR84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>4</v>
       </c>
@@ -7085,8 +7469,14 @@
       <c r="AP85">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ85">
+        <v>4</v>
+      </c>
+      <c r="AR85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>4</v>
       </c>
@@ -7157,8 +7547,14 @@
       <c r="AP86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ86">
+        <v>7</v>
+      </c>
+      <c r="AR86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>3</v>
       </c>
@@ -7253,8 +7649,14 @@
       <c r="AP87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ87">
+        <v>5</v>
+      </c>
+      <c r="AR87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>3</v>
       </c>
@@ -7334,8 +7736,14 @@
       <c r="AP88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ88">
+        <v>6</v>
+      </c>
+      <c r="AR88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>3</v>
       </c>
@@ -7397,8 +7805,11 @@
       <c r="AO89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>3</v>
       </c>
@@ -7460,8 +7871,11 @@
       <c r="AO90">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>1</v>
       </c>
@@ -7550,8 +7964,14 @@
       <c r="AP91">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ91">
+        <v>5</v>
+      </c>
+      <c r="AR91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>1</v>
       </c>
@@ -7619,8 +8039,14 @@
       <c r="AP92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ92">
+        <v>5</v>
+      </c>
+      <c r="AR92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>1</v>
       </c>
@@ -7682,8 +8108,11 @@
       <c r="AO93">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>1</v>
       </c>
@@ -7748,8 +8177,11 @@
       <c r="AO94">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>4</v>
       </c>
@@ -7808,8 +8240,11 @@
       <c r="AO95">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>4</v>
       </c>
@@ -7883,8 +8318,14 @@
       <c r="AP96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ96">
+        <v>9</v>
+      </c>
+      <c r="AR96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>4</v>
       </c>
@@ -7946,8 +8387,11 @@
       <c r="AO97">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>4</v>
       </c>
@@ -8021,8 +8465,14 @@
       <c r="AO98">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ98">
+        <v>6</v>
+      </c>
+      <c r="AR98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>3</v>
       </c>
@@ -8078,8 +8528,11 @@
       <c r="AO99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>3</v>
       </c>
@@ -8138,8 +8591,11 @@
       <c r="AO100">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>3</v>
       </c>
@@ -8201,8 +8657,14 @@
       <c r="AO101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ101">
+        <v>2</v>
+      </c>
+      <c r="AR101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>3</v>
       </c>
@@ -8264,8 +8726,11 @@
       <c r="AO102">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>1</v>
       </c>
@@ -8348,8 +8813,14 @@
       <c r="AP103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ103">
+        <v>4</v>
+      </c>
+      <c r="AR103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>1</v>
       </c>
@@ -8405,8 +8876,14 @@
       <c r="AP104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ104">
+        <v>7</v>
+      </c>
+      <c r="AR104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>1</v>
       </c>
@@ -8474,8 +8951,14 @@
       <c r="AP105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ105">
+        <v>4</v>
+      </c>
+      <c r="AR105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>1</v>
       </c>
@@ -8564,8 +9047,14 @@
       <c r="AP106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ106">
+        <v>6</v>
+      </c>
+      <c r="AR106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>4</v>
       </c>
@@ -8645,8 +9134,14 @@
       <c r="AP107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ107">
+        <v>4</v>
+      </c>
+      <c r="AR107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>4</v>
       </c>
@@ -8702,8 +9197,11 @@
       <c r="AO108">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>4</v>
       </c>
@@ -8771,8 +9269,14 @@
       <c r="AP109">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ109">
+        <v>1</v>
+      </c>
+      <c r="AR109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>4</v>
       </c>
@@ -8852,8 +9356,14 @@
       <c r="AP110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ110">
+        <v>6</v>
+      </c>
+      <c r="AR110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>3</v>
       </c>
@@ -8915,8 +9425,11 @@
       <c r="AO111">
         <v>6</v>
       </c>
-    </row>
-    <row r="112" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ111">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>3</v>
       </c>
@@ -8990,8 +9503,14 @@
       <c r="AP112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ112">
+        <v>7</v>
+      </c>
+      <c r="AR112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>3</v>
       </c>
@@ -9080,8 +9599,14 @@
       <c r="AP113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ113">
+        <v>4</v>
+      </c>
+      <c r="AR113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>3</v>
       </c>
@@ -9143,8 +9668,11 @@
       <c r="AO114">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>1</v>
       </c>
@@ -9236,8 +9764,14 @@
       <c r="AP115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ115">
+        <v>2</v>
+      </c>
+      <c r="AR115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>1</v>
       </c>
@@ -9293,8 +9827,14 @@
       <c r="AP116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ116">
+        <v>8</v>
+      </c>
+      <c r="AR116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>1</v>
       </c>
@@ -9362,8 +9902,14 @@
       <c r="AP117">
         <v>2</v>
       </c>
-    </row>
-    <row r="118" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ117">
+        <v>1</v>
+      </c>
+      <c r="AR117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>1</v>
       </c>
@@ -9429,8 +9975,11 @@
       <c r="AO118">
         <v>6</v>
       </c>
-    </row>
-    <row r="119" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>4</v>
       </c>
@@ -9486,8 +10035,11 @@
       <c r="AO119">
         <v>7</v>
       </c>
-    </row>
-    <row r="120" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ119">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>4</v>
       </c>
@@ -9546,8 +10098,11 @@
       <c r="AO120">
         <v>10</v>
       </c>
-    </row>
-    <row r="121" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ120">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>4</v>
       </c>
@@ -9609,8 +10164,11 @@
       <c r="AO121">
         <v>7</v>
       </c>
-    </row>
-    <row r="122" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ121">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>4</v>
       </c>
@@ -9675,8 +10233,11 @@
       <c r="AO122">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -9747,8 +10308,14 @@
       <c r="AP123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ123">
+        <v>3</v>
+      </c>
+      <c r="AR123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>3</v>
       </c>
@@ -9846,8 +10413,14 @@
       <c r="AP124">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ124">
+        <v>7</v>
+      </c>
+      <c r="AR124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>3</v>
       </c>
@@ -9945,8 +10518,14 @@
       <c r="AP125">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ125">
+        <v>0</v>
+      </c>
+      <c r="AR125">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>3</v>
       </c>
@@ -10023,8 +10602,14 @@
       <c r="AP126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ126">
+        <v>5</v>
+      </c>
+      <c r="AR126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>1</v>
       </c>
@@ -10098,8 +10683,14 @@
       <c r="AP127">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ127">
+        <v>2</v>
+      </c>
+      <c r="AR127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>1</v>
       </c>
@@ -10152,8 +10743,11 @@
       <c r="AO128">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ128">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>1</v>
       </c>
@@ -10227,8 +10821,14 @@
       <c r="AP129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ129">
+        <v>2</v>
+      </c>
+      <c r="AR129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>1</v>
       </c>
@@ -10293,8 +10893,11 @@
       <c r="AO130">
         <v>7</v>
       </c>
-    </row>
-    <row r="131" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ130">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>4</v>
       </c>
@@ -10359,8 +10962,14 @@
       <c r="AP131">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ131">
+        <v>7</v>
+      </c>
+      <c r="AR131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>4</v>
       </c>
@@ -10416,8 +11025,11 @@
       <c r="AO132">
         <v>6</v>
       </c>
-    </row>
-    <row r="133" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>4</v>
       </c>
@@ -10476,8 +11088,11 @@
       <c r="AO133">
         <v>6</v>
       </c>
-    </row>
-    <row r="134" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
         <v>4</v>
       </c>
@@ -10545,8 +11160,11 @@
       <c r="AO134">
         <v>10</v>
       </c>
-    </row>
-    <row r="135" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ134">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
         <v>3</v>
       </c>
@@ -10605,8 +11223,11 @@
       <c r="AO135">
         <v>7</v>
       </c>
-    </row>
-    <row r="136" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ135">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
         <v>3</v>
       </c>
@@ -10665,8 +11286,11 @@
       <c r="AO136">
         <v>6</v>
       </c>
-    </row>
-    <row r="137" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ136">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
         <v>3</v>
       </c>
@@ -10728,8 +11352,14 @@
       <c r="AO137">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ137">
+        <v>3</v>
+      </c>
+      <c r="AR137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
         <v>3</v>
       </c>
@@ -10809,8 +11439,14 @@
       <c r="AP138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ138">
+        <v>7</v>
+      </c>
+      <c r="AR138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
         <v>1</v>
       </c>
@@ -10872,8 +11508,14 @@
       <c r="AP139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ139">
+        <v>5</v>
+      </c>
+      <c r="AR139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
         <v>1</v>
       </c>
@@ -10926,8 +11568,11 @@
       <c r="AO140">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ140">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
         <v>1</v>
       </c>
@@ -11028,8 +11673,14 @@
       <c r="AP141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ141">
+        <v>4</v>
+      </c>
+      <c r="AR141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>1</v>
       </c>
@@ -11127,8 +11778,14 @@
       <c r="AP142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ142">
+        <v>6</v>
+      </c>
+      <c r="AR142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>4</v>
       </c>
@@ -11181,8 +11838,11 @@
       <c r="AO143">
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ143">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>4</v>
       </c>
@@ -11238,8 +11898,11 @@
       <c r="AO144">
         <v>7</v>
       </c>
-    </row>
-    <row r="145" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ144">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>4</v>
       </c>
@@ -11301,8 +11964,11 @@
       <c r="AO145">
         <v>7</v>
       </c>
-    </row>
-    <row r="146" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ145">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>4</v>
       </c>
@@ -11391,8 +12057,14 @@
       <c r="AP146">
         <v>2</v>
       </c>
-    </row>
-    <row r="147" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ146">
+        <v>8</v>
+      </c>
+      <c r="AR146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>3</v>
       </c>
@@ -11475,8 +12147,14 @@
       <c r="AP147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ147">
+        <v>2</v>
+      </c>
+      <c r="AR147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>3</v>
       </c>
@@ -11535,8 +12213,11 @@
       <c r="AO148">
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>3</v>
       </c>
@@ -11610,8 +12291,14 @@
       <c r="AP149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ149">
+        <v>2</v>
+      </c>
+      <c r="AR149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>3</v>
       </c>
@@ -11706,8 +12393,14 @@
       <c r="AP150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ150">
+        <v>8</v>
+      </c>
+      <c r="AR150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
         <v>1</v>
       </c>
@@ -11763,8 +12456,11 @@
       <c r="AO151">
         <v>7</v>
       </c>
-    </row>
-    <row r="152" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
         <v>1</v>
       </c>
@@ -11817,8 +12513,11 @@
       <c r="AO152">
         <v>9</v>
       </c>
-    </row>
-    <row r="153" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ152">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
         <v>1</v>
       </c>
@@ -11883,8 +12582,11 @@
       <c r="AO153">
         <v>6</v>
       </c>
-    </row>
-    <row r="154" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ153">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
         <v>1</v>
       </c>
@@ -11988,8 +12690,14 @@
       <c r="AP154">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ154">
+        <v>4</v>
+      </c>
+      <c r="AR154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
         <v>4</v>
       </c>
@@ -12060,8 +12768,14 @@
       <c r="AP155">
         <v>3</v>
       </c>
-    </row>
-    <row r="156" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ155">
+        <v>6</v>
+      </c>
+      <c r="AR155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
         <v>4</v>
       </c>
@@ -12120,8 +12834,11 @@
       <c r="AO156">
         <v>6</v>
       </c>
-    </row>
-    <row r="157" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ156">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
         <v>4</v>
       </c>
@@ -12183,8 +12900,11 @@
       <c r="AO157">
         <v>5</v>
       </c>
-    </row>
-    <row r="158" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ157">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B158" t="s">
         <v>4</v>
       </c>
@@ -12252,8 +12972,11 @@
       <c r="AO158">
         <v>7</v>
       </c>
-    </row>
-    <row r="159" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ158">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B159" t="s">
         <v>3</v>
       </c>
@@ -12324,8 +13047,14 @@
       <c r="AP159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ159">
+        <v>4</v>
+      </c>
+      <c r="AR159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B160" t="s">
         <v>3</v>
       </c>
@@ -12384,8 +13113,11 @@
       <c r="AO160">
         <v>9</v>
       </c>
-    </row>
-    <row r="161" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ160">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B161" t="s">
         <v>3</v>
       </c>
@@ -12480,8 +13212,14 @@
       <c r="AP161">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ161">
+        <v>2</v>
+      </c>
+      <c r="AR161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
         <v>3</v>
       </c>
@@ -12543,8 +13281,11 @@
       <c r="AO162">
         <v>8</v>
       </c>
-    </row>
-    <row r="163" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ162">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>1</v>
       </c>
@@ -12612,8 +13353,14 @@
       <c r="AP163">
         <v>3</v>
       </c>
-    </row>
-    <row r="164" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ163">
+        <v>5</v>
+      </c>
+      <c r="AR163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>1</v>
       </c>
@@ -12666,8 +13413,11 @@
       <c r="AO164">
         <v>9</v>
       </c>
-    </row>
-    <row r="165" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ164">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>1</v>
       </c>
@@ -12735,8 +13485,14 @@
       <c r="AP165">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ165">
+        <v>4</v>
+      </c>
+      <c r="AR165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>1</v>
       </c>
@@ -12825,8 +13581,14 @@
       <c r="AP166">
         <v>2</v>
       </c>
-    </row>
-    <row r="167" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ166">
+        <v>5</v>
+      </c>
+      <c r="AR166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
         <v>4</v>
       </c>
@@ -12882,8 +13644,14 @@
       <c r="AP167">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ167">
+        <v>7</v>
+      </c>
+      <c r="AR167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
         <v>4</v>
       </c>
@@ -12957,8 +13725,14 @@
       <c r="AP168">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ168">
+        <v>9</v>
+      </c>
+      <c r="AR168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B169" t="s">
         <v>4</v>
       </c>
@@ -13020,8 +13794,11 @@
       <c r="AO169">
         <v>6</v>
       </c>
-    </row>
-    <row r="170" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ169">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
         <v>4</v>
       </c>
@@ -13083,8 +13860,11 @@
       <c r="AO170">
         <v>7</v>
       </c>
-    </row>
-    <row r="171" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ170">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
         <v>3</v>
       </c>
@@ -13164,8 +13944,14 @@
       <c r="AP171">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ171">
+        <v>6</v>
+      </c>
+      <c r="AR171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
         <v>3</v>
       </c>
@@ -13224,8 +14010,11 @@
       <c r="AO172">
         <v>8</v>
       </c>
-    </row>
-    <row r="173" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ172">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
         <v>3</v>
       </c>
@@ -13284,8 +14073,11 @@
       <c r="AO173">
         <v>6</v>
       </c>
-    </row>
-    <row r="174" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ173">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B174" t="s">
         <v>3</v>
       </c>
@@ -13347,8 +14139,11 @@
       <c r="AO174">
         <v>9</v>
       </c>
-    </row>
-    <row r="175" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AQ174">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
         <v>1</v>
       </c>
@@ -13416,8 +14211,14 @@
       <c r="AP175">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ175">
+        <v>8</v>
+      </c>
+      <c r="AR175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
         <v>1</v>
       </c>
@@ -13470,8 +14271,11 @@
       <c r="AO176">
         <v>8</v>
       </c>
-    </row>
-    <row r="177" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ176">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
         <v>1</v>
       </c>
@@ -13530,8 +14334,11 @@
       <c r="AO177">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
         <v>1</v>
       </c>
@@ -13596,8 +14403,11 @@
       <c r="AO178">
         <v>8</v>
       </c>
-    </row>
-    <row r="179" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ178">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B179" t="s">
         <v>4</v>
       </c>
@@ -13668,8 +14478,14 @@
       <c r="AP179">
         <v>3</v>
       </c>
-    </row>
-    <row r="180" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ179">
+        <v>7</v>
+      </c>
+      <c r="AR179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B180" t="s">
         <v>4</v>
       </c>
@@ -13734,8 +14550,14 @@
       <c r="AP180">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ180">
+        <v>8</v>
+      </c>
+      <c r="AR180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
         <v>4</v>
       </c>
@@ -13794,8 +14616,14 @@
       <c r="AO181">
         <v>7</v>
       </c>
-    </row>
-    <row r="182" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ181">
+        <v>5</v>
+      </c>
+      <c r="AR181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
         <v>4</v>
       </c>
@@ -13857,8 +14685,11 @@
       <c r="AO182">
         <v>6</v>
       </c>
-    </row>
-    <row r="183" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ182">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
         <v>3</v>
       </c>
@@ -13943,8 +14774,14 @@
       <c r="AP183">
         <v>2</v>
       </c>
-    </row>
-    <row r="184" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ183">
+        <v>5</v>
+      </c>
+      <c r="AR183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
         <v>1</v>
       </c>
@@ -14002,8 +14839,11 @@
       <c r="AO184">
         <v>6</v>
       </c>
-    </row>
-    <row r="185" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ184">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
         <v>3</v>
       </c>
@@ -14061,8 +14901,14 @@
       <c r="AO185">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ185">
+        <v>3</v>
+      </c>
+      <c r="AR185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
         <v>1</v>
       </c>
@@ -14126,8 +14972,14 @@
       <c r="AP186">
         <v>1</v>
       </c>
-    </row>
-    <row r="187" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ186">
+        <v>6</v>
+      </c>
+      <c r="AR186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
         <v>4</v>
       </c>
@@ -14182,8 +15034,11 @@
       <c r="AO187">
         <v>7</v>
       </c>
-    </row>
-    <row r="188" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ187">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="188" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
         <v>4</v>
       </c>
@@ -14250,8 +15105,14 @@
       <c r="AP188">
         <v>2</v>
       </c>
-    </row>
-    <row r="189" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ188">
+        <v>8</v>
+      </c>
+      <c r="AR188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
         <v>3</v>
       </c>
@@ -14342,8 +15203,14 @@
       <c r="AP189">
         <v>2</v>
       </c>
-    </row>
-    <row r="190" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ189">
+        <v>2</v>
+      </c>
+      <c r="AR189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
         <v>1</v>
       </c>
@@ -14425,8 +15292,14 @@
       <c r="AP190">
         <v>2</v>
       </c>
-    </row>
-    <row r="191" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ190">
+        <v>3</v>
+      </c>
+      <c r="AR190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
         <v>3</v>
       </c>
@@ -14508,8 +15381,14 @@
       <c r="AP191">
         <v>2</v>
       </c>
-    </row>
-    <row r="192" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ191">
+        <v>1</v>
+      </c>
+      <c r="AR191">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
         <v>1</v>
       </c>
@@ -14576,8 +15455,14 @@
       <c r="AP192">
         <v>2</v>
       </c>
-    </row>
-    <row r="193" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ192">
+        <v>1</v>
+      </c>
+      <c r="AR192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B193" t="s">
         <v>4</v>
       </c>
@@ -14665,8 +15550,14 @@
       <c r="AP193">
         <v>3</v>
       </c>
-    </row>
-    <row r="194" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ193">
+        <v>4</v>
+      </c>
+      <c r="AR193">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B194" t="s">
         <v>4</v>
       </c>
@@ -14730,8 +15621,14 @@
       <c r="AP194">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ194">
+        <v>4</v>
+      </c>
+      <c r="AR194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B195" t="s">
         <v>3</v>
       </c>
@@ -14819,8 +15716,14 @@
       <c r="AP195">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ195">
+        <v>2</v>
+      </c>
+      <c r="AR195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B196" t="s">
         <v>1</v>
       </c>
@@ -14914,8 +15817,14 @@
       <c r="AP196">
         <v>3</v>
       </c>
-    </row>
-    <row r="197" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ196">
+        <v>5</v>
+      </c>
+      <c r="AR196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B197" t="s">
         <v>3</v>
       </c>
@@ -14982,8 +15891,14 @@
       <c r="AO197">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ197">
+        <v>3</v>
+      </c>
+      <c r="AR197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B198" t="s">
         <v>1</v>
       </c>
@@ -15041,8 +15956,11 @@
       <c r="AO198">
         <v>5</v>
       </c>
-    </row>
-    <row r="199" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ198">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B199" t="s">
         <v>4</v>
       </c>
@@ -15115,8 +16033,14 @@
       <c r="AP199">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ199">
+        <v>5</v>
+      </c>
+      <c r="AR199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B200" t="s">
         <v>4</v>
       </c>
@@ -15177,8 +16101,11 @@
       <c r="AO200">
         <v>7</v>
       </c>
-    </row>
-    <row r="201" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ200">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B201" t="s">
         <v>3</v>
       </c>
@@ -15257,8 +16184,14 @@
       <c r="AP201">
         <v>2</v>
       </c>
-    </row>
-    <row r="202" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ201">
+        <v>3</v>
+      </c>
+      <c r="AR201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B202" t="s">
         <v>1</v>
       </c>
@@ -15346,8 +16279,14 @@
       <c r="AP202">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ202">
+        <v>0</v>
+      </c>
+      <c r="AR202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B203" t="s">
         <v>3</v>
       </c>
@@ -15420,8 +16359,14 @@
       <c r="AP203">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ203">
+        <v>2</v>
+      </c>
+      <c r="AR203">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B204" t="s">
         <v>1</v>
       </c>
@@ -15479,8 +16424,11 @@
       <c r="AO204">
         <v>5</v>
       </c>
-    </row>
-    <row r="205" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ204">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B205" t="s">
         <v>4</v>
       </c>
@@ -15571,8 +16519,14 @@
       <c r="AP205">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ205">
+        <v>9</v>
+      </c>
+      <c r="AR205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
         <v>4</v>
       </c>
@@ -15630,8 +16584,11 @@
       <c r="AO206">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ206">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
         <v>3</v>
       </c>
@@ -15689,8 +16646,11 @@
       <c r="AO207">
         <v>4</v>
       </c>
-    </row>
-    <row r="208" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B208" t="s">
         <v>1</v>
       </c>
@@ -15772,8 +16732,14 @@
       <c r="AP208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ208">
+        <v>2</v>
+      </c>
+      <c r="AR208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B209" t="s">
         <v>3</v>
       </c>
@@ -15837,8 +16803,14 @@
       <c r="AP209">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ209">
+        <v>4</v>
+      </c>
+      <c r="AR209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B210" t="s">
         <v>1</v>
       </c>
@@ -15926,8 +16898,14 @@
       <c r="AP210">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ210">
+        <v>4</v>
+      </c>
+      <c r="AR210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B211" t="s">
         <v>4</v>
       </c>
@@ -15991,8 +16969,14 @@
       <c r="AP211">
         <v>2</v>
       </c>
-    </row>
-    <row r="212" spans="2:42" hidden="1" x14ac:dyDescent="0.35">
+      <c r="AQ211">
+        <v>3</v>
+      </c>
+      <c r="AR211">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B212" t="s">
         <v>4</v>
       </c>
@@ -16050,8 +17034,13 @@
       <c r="AO212">
         <v>5</v>
       </c>
-    </row>
-    <row r="213" spans="2:42" hidden="1" x14ac:dyDescent="0.35"/>
+      <c r="AQ212">
+        <v>4</v>
+      </c>
+      <c r="AR212">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>